<commit_message>
Version 03 | All ICE Index Comparisons in a single file
</commit_message>
<xml_diff>
--- a/Static Data/ISINtoTicker.xlsx
+++ b/Static Data/ISINtoTicker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sahilkhan/Downloads/Rebalance Project/Static Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17328CF-1E29-D24C-8613-898828E3003D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9A6164-D244-134D-94CC-65C0F353D58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="760" windowWidth="26700" windowHeight="18880" xr2:uid="{88480EA4-891F-3C45-B324-C2A159DC6245}"/>
+    <workbookView xWindow="3540" yWindow="760" windowWidth="17300" windowHeight="18880" xr2:uid="{88480EA4-891F-3C45-B324-C2A159DC6245}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="1437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="1443">
   <si>
     <t>ISIN</t>
   </si>
@@ -4346,6 +4346,24 @@
   </si>
   <si>
     <t>Last Price</t>
+  </si>
+  <si>
+    <t>ASBA</t>
+  </si>
+  <si>
+    <t>US0454876006</t>
+  </si>
+  <si>
+    <t>HBANL</t>
+  </si>
+  <si>
+    <t>US2263443077</t>
+  </si>
+  <si>
+    <t>CEQP.PR</t>
+  </si>
+  <si>
+    <t>US4461507737</t>
   </si>
 </sst>
 </file>
@@ -4536,8 +4554,8 @@
         <stp>realtime</stp>
         <stp>RILYG</stp>
         <stp>Last(0,12;0,113)</stp>
+        <tr r="E682" s="1"/>
         <tr r="E386" s="1"/>
-        <tr r="E682" s="1"/>
       </tp>
       <tp t="e">
         <v>#N/A</v>
@@ -4882,8 +4900,8 @@
         <stp>realtime</stp>
         <stp>GBLL</stp>
         <stp>Last(0,12;0,113)</stp>
+        <tr r="E526" s="1"/>
         <tr r="E226" s="1"/>
-        <tr r="E526" s="1"/>
       </tp>
       <tp t="e">
         <v>#N/A</v>
@@ -5089,9 +5107,25 @@
         <v>#N/A</v>
         <stp/>
         <stp>realtime</stp>
+        <stp>CEQPp</stp>
+        <stp>Last(0,12;0,113)</stp>
+        <tr r="E719" s="1"/>
+      </tp>
+      <tp t="e">
+        <v>#N/A</v>
+        <stp/>
+        <stp>realtime</stp>
         <stp>CTBB</stp>
         <stp>Last(0,12;0,113)</stp>
         <tr r="E151" s="1"/>
+      </tp>
+      <tp t="e">
+        <v>#N/A</v>
+        <stp/>
+        <stp>realtime</stp>
+        <stp>ASBA</stp>
+        <stp>Last(0,12;0,113)</stp>
+        <tr r="E717" s="1"/>
       </tp>
       <tp t="e">
         <v>#N/A</v>
@@ -5716,8 +5750,8 @@
         <stp>realtime</stp>
         <stp>DCOMP</stp>
         <stp>Last(0,12;0,113)</stp>
+        <tr r="E572" s="1"/>
         <tr r="E156" s="1"/>
-        <tr r="E572" s="1"/>
       </tp>
       <tp t="e">
         <v>#N/A</v>
@@ -5798,6 +5832,14 @@
         <stp>HBANM</stp>
         <stp>Last(0,12;0,113)</stp>
         <tr r="E615" s="1"/>
+      </tp>
+      <tp t="e">
+        <v>#N/A</v>
+        <stp/>
+        <stp>realtime</stp>
+        <stp>HBANL</stp>
+        <stp>Last(0,12;0,113)</stp>
+        <tr r="E718" s="1"/>
       </tp>
       <tp t="e">
         <v>#N/A</v>
@@ -10409,8 +10451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72855C2C-66C1-AE40-9867-C6069708BE15}">
   <dimension ref="A1:F1392"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A699" zoomScale="186" workbookViewId="0">
+      <selection activeCell="C716" sqref="C716"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10481,7 +10523,7 @@
         <v>#N/A</v>
       </c>
       <c r="F3">
-        <v>22.53</v>
+        <v>22.11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -10550,7 +10592,7 @@
         <v>#N/A</v>
       </c>
       <c r="F6">
-        <v>20.58</v>
+        <v>20.150500000000001</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -10573,7 +10615,7 @@
         <v>#N/A</v>
       </c>
       <c r="F7">
-        <v>22.25</v>
+        <v>21.67</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -10642,7 +10684,7 @@
         <v>#N/A</v>
       </c>
       <c r="F10">
-        <v>24.93</v>
+        <v>24.5657</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -10665,7 +10707,7 @@
         <v>#N/A</v>
       </c>
       <c r="F11">
-        <v>21.69</v>
+        <v>21.17</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -10688,7 +10730,7 @@
         <v>#N/A</v>
       </c>
       <c r="F12">
-        <v>23.41</v>
+        <v>23.01</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -10734,7 +10776,7 @@
         <v>#N/A</v>
       </c>
       <c r="F14">
-        <v>22.49</v>
+        <v>21.18</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -10757,7 +10799,7 @@
         <v>#N/A</v>
       </c>
       <c r="F15">
-        <v>23.1112</v>
+        <v>23.41</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -10780,7 +10822,7 @@
         <v>#N/A</v>
       </c>
       <c r="F16">
-        <v>22.62</v>
+        <v>22.59</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -10803,7 +10845,7 @@
         <v>#N/A</v>
       </c>
       <c r="F17">
-        <v>25.495000000000001</v>
+        <v>25.25</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -10826,7 +10868,7 @@
         <v>#N/A</v>
       </c>
       <c r="F18">
-        <v>22.31</v>
+        <v>21.82</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -10849,7 +10891,7 @@
         <v>#N/A</v>
       </c>
       <c r="F19">
-        <v>21.34</v>
+        <v>20.65</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -10941,7 +10983,7 @@
         <v>#N/A</v>
       </c>
       <c r="F23">
-        <v>25.02</v>
+        <v>24.7563</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -10964,7 +11006,7 @@
         <v>#N/A</v>
       </c>
       <c r="F24">
-        <v>21.87</v>
+        <v>20.97</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -10987,7 +11029,7 @@
         <v>#N/A</v>
       </c>
       <c r="F25">
-        <v>21.43</v>
+        <v>20.83</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -11010,7 +11052,7 @@
         <v>#N/A</v>
       </c>
       <c r="F26">
-        <v>17.39</v>
+        <v>17.059999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -11033,7 +11075,7 @@
         <v>#N/A</v>
       </c>
       <c r="F27">
-        <v>19.149999999999999</v>
+        <v>18.64</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -11056,7 +11098,7 @@
         <v>#N/A</v>
       </c>
       <c r="F28">
-        <v>17.38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -11079,7 +11121,7 @@
         <v>#N/A</v>
       </c>
       <c r="F29">
-        <v>23.52</v>
+        <v>23.82</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -11125,7 +11167,7 @@
         <v>#N/A</v>
       </c>
       <c r="F31">
-        <v>24.2</v>
+        <v>24.05</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -11148,7 +11190,7 @@
         <v>#N/A</v>
       </c>
       <c r="F32">
-        <v>24.38</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -11240,7 +11282,7 @@
         <v>#N/A</v>
       </c>
       <c r="F36">
-        <v>25.58</v>
+        <v>25.55</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -11263,7 +11305,7 @@
         <v>#N/A</v>
       </c>
       <c r="F37">
-        <v>25.16</v>
+        <v>25.210100000000001</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -11286,7 +11328,7 @@
         <v>#N/A</v>
       </c>
       <c r="F38">
-        <v>22.57</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -11309,7 +11351,7 @@
         <v>#N/A</v>
       </c>
       <c r="F39">
-        <v>21.85</v>
+        <v>21.49</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -11447,7 +11489,7 @@
         <v>#N/A</v>
       </c>
       <c r="F45">
-        <v>23.36</v>
+        <v>22.49</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -11470,7 +11512,7 @@
         <v>#N/A</v>
       </c>
       <c r="F46">
-        <v>24.65</v>
+        <v>23.55</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -11493,7 +11535,7 @@
         <v>#N/A</v>
       </c>
       <c r="F47">
-        <v>24.05</v>
+        <v>22.4101</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -11516,7 +11558,7 @@
         <v>#N/A</v>
       </c>
       <c r="F48">
-        <v>23.95</v>
+        <v>22.443200000000001</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -11539,7 +11581,7 @@
         <v>#N/A</v>
       </c>
       <c r="F49">
-        <v>129.37</v>
+        <v>124.88</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -11562,7 +11604,7 @@
         <v>#N/A</v>
       </c>
       <c r="F50">
-        <v>24.37</v>
+        <v>23.84</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -11585,7 +11627,7 @@
         <v>#N/A</v>
       </c>
       <c r="F51">
-        <v>23.24</v>
+        <v>23.16</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -11631,7 +11673,7 @@
         <v>#N/A</v>
       </c>
       <c r="F53">
-        <v>22.15</v>
+        <v>21.9</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -11654,7 +11696,7 @@
         <v>#N/A</v>
       </c>
       <c r="F54">
-        <v>20.75</v>
+        <v>20.700099999999999</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -11677,7 +11719,7 @@
         <v>#N/A</v>
       </c>
       <c r="F55">
-        <v>24.35</v>
+        <v>23.6</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -11700,7 +11742,7 @@
         <v>#N/A</v>
       </c>
       <c r="F56">
-        <v>22.76</v>
+        <v>22.6</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -11723,7 +11765,7 @@
         <v>#N/A</v>
       </c>
       <c r="F57">
-        <v>23.33</v>
+        <v>23.14</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -11792,7 +11834,7 @@
         <v>#N/A</v>
       </c>
       <c r="F60">
-        <v>22.5</v>
+        <v>21.59</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -11838,7 +11880,7 @@
         <v>#N/A</v>
       </c>
       <c r="F62">
-        <v>24.75</v>
+        <v>23.82</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -11861,7 +11903,7 @@
         <v>#N/A</v>
       </c>
       <c r="F63">
-        <v>21.5</v>
+        <v>21.07</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -11884,7 +11926,7 @@
         <v>#N/A</v>
       </c>
       <c r="F64">
-        <v>25.18</v>
+        <v>25.01</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -11907,7 +11949,7 @@
         <v>#N/A</v>
       </c>
       <c r="F65">
-        <v>25.54</v>
+        <v>24.83</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -11976,7 +12018,7 @@
         <v>#N/A</v>
       </c>
       <c r="F68">
-        <v>21.76</v>
+        <v>21.695</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -12022,7 +12064,7 @@
         <v>#N/A</v>
       </c>
       <c r="F70">
-        <v>24.98</v>
+        <v>24.76</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -12068,7 +12110,7 @@
         <v>#N/A</v>
       </c>
       <c r="F72">
-        <v>20.96</v>
+        <v>21.32</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -12091,7 +12133,7 @@
         <v>#N/A</v>
       </c>
       <c r="F73">
-        <v>24.89</v>
+        <v>24.38</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -12114,7 +12156,7 @@
         <v>#N/A</v>
       </c>
       <c r="F74">
-        <v>1185.9000000000001</v>
+        <v>1182.07</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -12137,7 +12179,7 @@
         <v>#N/A</v>
       </c>
       <c r="F75">
-        <v>23.01</v>
+        <v>22.21</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -12160,7 +12202,7 @@
         <v>#N/A</v>
       </c>
       <c r="F76">
-        <v>21.6</v>
+        <v>20.88</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -12206,7 +12248,7 @@
         <v>#N/A</v>
       </c>
       <c r="F78">
-        <v>25.572099999999999</v>
+        <v>24.67</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -12229,7 +12271,7 @@
         <v>#N/A</v>
       </c>
       <c r="F79">
-        <v>25.2</v>
+        <v>25.23</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -12252,7 +12294,7 @@
         <v>#N/A</v>
       </c>
       <c r="F80">
-        <v>25.37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -12275,7 +12317,7 @@
         <v>#N/A</v>
       </c>
       <c r="F81">
-        <v>48</v>
+        <v>48.24</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -12298,7 +12340,7 @@
         <v>#N/A</v>
       </c>
       <c r="F82">
-        <v>20.399999999999999</v>
+        <v>18.75</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -12321,7 +12363,7 @@
         <v>#N/A</v>
       </c>
       <c r="F83">
-        <v>21.95</v>
+        <v>20.91</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -12344,7 +12386,7 @@
         <v>#N/A</v>
       </c>
       <c r="F84">
-        <v>24.452300000000001</v>
+        <v>23.84</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -12367,7 +12409,7 @@
         <v>#N/A</v>
       </c>
       <c r="F85">
-        <v>25.25</v>
+        <v>24.3</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -12390,7 +12432,7 @@
         <v>#N/A</v>
       </c>
       <c r="F86">
-        <v>25.19</v>
+        <v>24.15</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -12413,7 +12455,7 @@
         <v>#N/A</v>
       </c>
       <c r="F87">
-        <v>17.36</v>
+        <v>16.16</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -12482,7 +12524,7 @@
         <v>#N/A</v>
       </c>
       <c r="F90">
-        <v>20.78</v>
+        <v>20.67</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
@@ -12505,7 +12547,7 @@
         <v>#N/A</v>
       </c>
       <c r="F91">
-        <v>21.07</v>
+        <v>21.08</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -12528,7 +12570,7 @@
         <v>#N/A</v>
       </c>
       <c r="F92">
-        <v>20.93</v>
+        <v>20.97</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
@@ -12574,7 +12616,7 @@
         <v>#N/A</v>
       </c>
       <c r="F94">
-        <v>25.01</v>
+        <v>24.73</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
@@ -12620,7 +12662,7 @@
         <v>#N/A</v>
       </c>
       <c r="F96">
-        <v>17.0442</v>
+        <v>14.855</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
@@ -12643,7 +12685,7 @@
         <v>#N/A</v>
       </c>
       <c r="F97">
-        <v>17.97</v>
+        <v>15.94</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
@@ -12666,7 +12708,7 @@
         <v>#N/A</v>
       </c>
       <c r="F98">
-        <v>18.75</v>
+        <v>16.850000000000001</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
@@ -12758,7 +12800,7 @@
         <v>#N/A</v>
       </c>
       <c r="F102">
-        <v>113.61</v>
+        <v>113.64</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
@@ -12804,7 +12846,7 @@
         <v>#N/A</v>
       </c>
       <c r="F104">
-        <v>25.48</v>
+        <v>25.45</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
@@ -12827,7 +12869,7 @@
         <v>#N/A</v>
       </c>
       <c r="F105">
-        <v>25.18</v>
+        <v>25.156600000000001</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
@@ -12850,7 +12892,7 @@
         <v>#N/A</v>
       </c>
       <c r="F106">
-        <v>28.28</v>
+        <v>27.84</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
@@ -12988,7 +13030,7 @@
         <v>#N/A</v>
       </c>
       <c r="F112">
-        <v>11.79</v>
+        <v>11.909700000000001</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
@@ -13011,7 +13053,7 @@
         <v>#N/A</v>
       </c>
       <c r="F113">
-        <v>25.52</v>
+        <v>25.030100000000001</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
@@ -13034,7 +13076,7 @@
         <v>#N/A</v>
       </c>
       <c r="F114">
-        <v>20.98</v>
+        <v>20.39</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -13057,7 +13099,7 @@
         <v>#N/A</v>
       </c>
       <c r="F115">
-        <v>108.58</v>
+        <v>100.94</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
@@ -13126,7 +13168,7 @@
         <v>#N/A</v>
       </c>
       <c r="F118">
-        <v>26.25</v>
+        <v>25.82</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
@@ -13149,7 +13191,7 @@
         <v>#N/A</v>
       </c>
       <c r="F119">
-        <v>25.45</v>
+        <v>25.4</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -13172,7 +13214,7 @@
         <v>#N/A</v>
       </c>
       <c r="F120">
-        <v>25.41</v>
+        <v>25.405000000000001</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
@@ -13195,7 +13237,7 @@
         <v>#N/A</v>
       </c>
       <c r="F121">
-        <v>25.99</v>
+        <v>25.92</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
@@ -13218,7 +13260,7 @@
         <v>#N/A</v>
       </c>
       <c r="F122">
-        <v>29.6</v>
+        <v>29.55</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
@@ -13241,7 +13283,7 @@
         <v>#N/A</v>
       </c>
       <c r="F123">
-        <v>21.14</v>
+        <v>20.63</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
@@ -13264,7 +13306,7 @@
         <v>#N/A</v>
       </c>
       <c r="F124">
-        <v>22.11</v>
+        <v>21.26</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
@@ -13287,7 +13329,7 @@
         <v>#N/A</v>
       </c>
       <c r="F125">
-        <v>19.64</v>
+        <v>19.5899</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
@@ -13310,7 +13352,7 @@
         <v>#N/A</v>
       </c>
       <c r="F126">
-        <v>21.2</v>
+        <v>20.67</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
@@ -13333,7 +13375,7 @@
         <v>#N/A</v>
       </c>
       <c r="F127">
-        <v>19.6541</v>
+        <v>18.34</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
@@ -13471,7 +13513,7 @@
         <v>#N/A</v>
       </c>
       <c r="F133">
-        <v>23.3</v>
+        <v>23.242100000000001</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
@@ -13494,7 +13536,7 @@
         <v>#N/A</v>
       </c>
       <c r="F134">
-        <v>24.315000000000001</v>
+        <v>23.95</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
@@ -13517,7 +13559,7 @@
         <v>#N/A</v>
       </c>
       <c r="F135">
-        <v>24.35</v>
+        <v>23.67</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
@@ -13563,7 +13605,7 @@
         <v>#N/A</v>
       </c>
       <c r="F137">
-        <v>24.6</v>
+        <v>24.34</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
@@ -13586,7 +13628,7 @@
         <v>#N/A</v>
       </c>
       <c r="F138">
-        <v>24.782599999999999</v>
+        <v>24.76</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
@@ -13609,7 +13651,7 @@
         <v>#N/A</v>
       </c>
       <c r="F139">
-        <v>24.65</v>
+        <v>24.7119</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
@@ -13701,7 +13743,7 @@
         <v>#N/A</v>
       </c>
       <c r="F143">
-        <v>20.78</v>
+        <v>20.209099999999999</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
@@ -13724,7 +13766,7 @@
         <v>#N/A</v>
       </c>
       <c r="F144">
-        <v>19.57</v>
+        <v>18.95</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
@@ -13747,7 +13789,7 @@
         <v>#N/A</v>
       </c>
       <c r="F145">
-        <v>5.01</v>
+        <v>5.07</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
@@ -13770,7 +13812,7 @@
         <v>#N/A</v>
       </c>
       <c r="F146" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
@@ -13839,7 +13881,7 @@
         <v>#N/A</v>
       </c>
       <c r="F149">
-        <v>89.01</v>
+        <v>89.7637</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
@@ -13885,7 +13927,7 @@
         <v>#N/A</v>
       </c>
       <c r="F151">
-        <v>17.66</v>
+        <v>17.29</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
@@ -13908,7 +13950,7 @@
         <v>#N/A</v>
       </c>
       <c r="F152">
-        <v>18.670000000000002</v>
+        <v>18.12</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
@@ -14000,7 +14042,7 @@
         <v>#N/A</v>
       </c>
       <c r="F156">
-        <v>20.350000000000001</v>
+        <v>18.760000000000002</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
@@ -14023,7 +14065,7 @@
         <v>#N/A</v>
       </c>
       <c r="F157">
-        <v>25.010200000000001</v>
+        <v>25.01</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
@@ -14046,7 +14088,7 @@
         <v>#N/A</v>
       </c>
       <c r="F158">
-        <v>25.41</v>
+        <v>25.22</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.2">
@@ -14092,7 +14134,7 @@
         <v>#N/A</v>
       </c>
       <c r="F160">
-        <v>25.4376</v>
+        <v>25.32</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
@@ -14115,7 +14157,7 @@
         <v>#N/A</v>
       </c>
       <c r="F161">
-        <v>12.9</v>
+        <v>13.25</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
@@ -14138,7 +14180,7 @@
         <v>#N/A</v>
       </c>
       <c r="F162">
-        <v>13.82</v>
+        <v>14.02</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.2">
@@ -14184,7 +14226,7 @@
         <v>#N/A</v>
       </c>
       <c r="F164">
-        <v>1264.9100000000001</v>
+        <v>1234.68</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.2">
@@ -14276,7 +14318,7 @@
         <v>#N/A</v>
       </c>
       <c r="F168">
-        <v>22.448</v>
+        <v>21.95</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
@@ -14299,7 +14341,7 @@
         <v>#N/A</v>
       </c>
       <c r="F169">
-        <v>24.18</v>
+        <v>23.549399999999999</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.2">
@@ -14322,7 +14364,7 @@
         <v>#N/A</v>
       </c>
       <c r="F170">
-        <v>22.13</v>
+        <v>21.79</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
@@ -14391,7 +14433,7 @@
         <v>#N/A</v>
       </c>
       <c r="F173">
-        <v>3.02</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.2">
@@ -14460,7 +14502,7 @@
         <v>#N/A</v>
       </c>
       <c r="F176">
-        <v>23.66</v>
+        <v>23.14</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
@@ -14506,7 +14548,7 @@
         <v>#N/A</v>
       </c>
       <c r="F178">
-        <v>25</v>
+        <v>24.497</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
@@ -14529,7 +14571,7 @@
         <v>#N/A</v>
       </c>
       <c r="F179">
-        <v>25.02</v>
+        <v>24.68</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
@@ -14575,7 +14617,7 @@
         <v>#N/A</v>
       </c>
       <c r="F181">
-        <v>22.5</v>
+        <v>22.61</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">
@@ -14644,7 +14686,7 @@
         <v>#N/A</v>
       </c>
       <c r="F184">
-        <v>22.29</v>
+        <v>21.31</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
@@ -14690,7 +14732,7 @@
         <v>#N/A</v>
       </c>
       <c r="F186">
-        <v>22.39</v>
+        <v>21.63</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.2">
@@ -14736,7 +14778,7 @@
         <v>#N/A</v>
       </c>
       <c r="F188">
-        <v>22.32</v>
+        <v>21.08</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.2">
@@ -14805,7 +14847,7 @@
         <v>#N/A</v>
       </c>
       <c r="F191">
-        <v>22.73</v>
+        <v>21.94</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.2">
@@ -14828,7 +14870,7 @@
         <v>#N/A</v>
       </c>
       <c r="F192">
-        <v>25.02</v>
+        <v>25.04</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.2">
@@ -14851,7 +14893,7 @@
         <v>#N/A</v>
       </c>
       <c r="F193">
-        <v>23.91</v>
+        <v>23.469899999999999</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.2">
@@ -14920,7 +14962,7 @@
         <v>#N/A</v>
       </c>
       <c r="F196">
-        <v>19.2285</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.2">
@@ -14943,7 +14985,7 @@
         <v>#N/A</v>
       </c>
       <c r="F197">
-        <v>28.123699999999999</v>
+        <v>28.07</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.2">
@@ -14966,7 +15008,7 @@
         <v>#N/A</v>
       </c>
       <c r="F198">
-        <v>19.47</v>
+        <v>18.3065</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.2">
@@ -14989,7 +15031,7 @@
         <v>#N/A</v>
       </c>
       <c r="F199">
-        <v>25.5</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.2">
@@ -15012,7 +15054,7 @@
         <v>#N/A</v>
       </c>
       <c r="F200">
-        <v>21.601875</v>
+        <v>20.84</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.2">
@@ -15035,7 +15077,7 @@
         <v>#N/A</v>
       </c>
       <c r="F201">
-        <v>24.23</v>
+        <v>23.81</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.2">
@@ -15058,7 +15100,7 @@
         <v>#N/A</v>
       </c>
       <c r="F202">
-        <v>23.6282</v>
+        <v>23.1662</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.2">
@@ -15173,7 +15215,7 @@
         <v>#N/A</v>
       </c>
       <c r="F207">
-        <v>24.09</v>
+        <v>23.8</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.2">
@@ -15196,7 +15238,7 @@
         <v>#N/A</v>
       </c>
       <c r="F208">
-        <v>23.9</v>
+        <v>23.3</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.2">
@@ -15219,7 +15261,7 @@
         <v>#N/A</v>
       </c>
       <c r="F209">
-        <v>21.95</v>
+        <v>21.79</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">
@@ -15265,7 +15307,7 @@
         <v>#N/A</v>
       </c>
       <c r="F211">
-        <v>24.76</v>
+        <v>24.28</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.2">
@@ -15288,7 +15330,7 @@
         <v>#N/A</v>
       </c>
       <c r="F212">
-        <v>24.92</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.2">
@@ -15311,7 +15353,7 @@
         <v>#N/A</v>
       </c>
       <c r="F213">
-        <v>25.16</v>
+        <v>25.06</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.2">
@@ -15334,7 +15376,7 @@
         <v>#N/A</v>
       </c>
       <c r="F214">
-        <v>22.37</v>
+        <v>21.86</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.2">
@@ -15357,7 +15399,7 @@
         <v>#N/A</v>
       </c>
       <c r="F215">
-        <v>24.47</v>
+        <v>23.53</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.2">
@@ -15380,7 +15422,7 @@
         <v>#N/A</v>
       </c>
       <c r="F216">
-        <v>25.72</v>
+        <v>25.24</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.2">
@@ -15472,7 +15514,7 @@
         <v>#N/A</v>
       </c>
       <c r="F220">
-        <v>20.97</v>
+        <v>20</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.2">
@@ -15495,7 +15537,7 @@
         <v>#N/A</v>
       </c>
       <c r="F221">
-        <v>23.062000000000001</v>
+        <v>21.68</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.2">
@@ -15518,7 +15560,7 @@
         <v>#N/A</v>
       </c>
       <c r="F222">
-        <v>19.73</v>
+        <v>18.71</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.2">
@@ -15541,7 +15583,7 @@
         <v>#N/A</v>
       </c>
       <c r="F223">
-        <v>21.88</v>
+        <v>21.2</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.2">
@@ -15564,7 +15606,7 @@
         <v>#N/A</v>
       </c>
       <c r="F224">
-        <v>22.860099999999999</v>
+        <v>22.113600000000002</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.2">
@@ -15633,7 +15675,7 @@
         <v>#N/A</v>
       </c>
       <c r="F227">
-        <v>66.75</v>
+        <v>71.56</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.2">
@@ -15702,7 +15744,7 @@
         <v>#N/A</v>
       </c>
       <c r="F230">
-        <v>24.8</v>
+        <v>24.930099999999999</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.2">
@@ -15771,7 +15813,7 @@
         <v>#N/A</v>
       </c>
       <c r="F233">
-        <v>22.5</v>
+        <v>21.72</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.2">
@@ -15794,7 +15836,7 @@
         <v>#N/A</v>
       </c>
       <c r="F234">
-        <v>22.95</v>
+        <v>22.7699</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.2">
@@ -15817,7 +15859,7 @@
         <v>#N/A</v>
       </c>
       <c r="F235">
-        <v>20.89</v>
+        <v>20.88</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.2">
@@ -15840,7 +15882,7 @@
         <v>#N/A</v>
       </c>
       <c r="F236">
-        <v>21.1</v>
+        <v>21.41</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.2">
@@ -15863,7 +15905,7 @@
         <v>#N/A</v>
       </c>
       <c r="F237">
-        <v>20.644200000000001</v>
+        <v>20.89</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.2">
@@ -15886,7 +15928,7 @@
         <v>#N/A</v>
       </c>
       <c r="F238">
-        <v>24.97</v>
+        <v>25.03</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.2">
@@ -15909,7 +15951,7 @@
         <v>#N/A</v>
       </c>
       <c r="F239">
-        <v>25.23</v>
+        <v>25.14</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.2">
@@ -16024,7 +16066,7 @@
         <v>#N/A</v>
       </c>
       <c r="F244">
-        <v>25.2</v>
+        <v>24.95</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.2">
@@ -16116,7 +16158,7 @@
         <v>#N/A</v>
       </c>
       <c r="F248">
-        <v>20.89</v>
+        <v>20.65</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.2">
@@ -16139,7 +16181,7 @@
         <v>#N/A</v>
       </c>
       <c r="F249">
-        <v>21.2</v>
+        <v>21.35</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.2">
@@ -16185,7 +16227,7 @@
         <v>#N/A</v>
       </c>
       <c r="F251">
-        <v>25</v>
+        <v>24.73</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.2">
@@ -16231,7 +16273,7 @@
         <v>#N/A</v>
       </c>
       <c r="F253">
-        <v>20.43</v>
+        <v>18.670000000000002</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.2">
@@ -16300,7 +16342,7 @@
         <v>#N/A</v>
       </c>
       <c r="F256">
-        <v>22.265599999999999</v>
+        <v>20.2</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.2">
@@ -16323,7 +16365,7 @@
         <v>#N/A</v>
       </c>
       <c r="F257">
-        <v>22.131250000000001</v>
+        <v>19.12</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.2">
@@ -16369,7 +16411,7 @@
         <v>#N/A</v>
       </c>
       <c r="F259">
-        <v>25.32</v>
+        <v>24.93</v>
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.2">
@@ -16392,7 +16434,7 @@
         <v>#N/A</v>
       </c>
       <c r="F260">
-        <v>24.87</v>
+        <v>24.35</v>
       </c>
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.2">
@@ -16461,7 +16503,7 @@
         <v>#N/A</v>
       </c>
       <c r="F263">
-        <v>20.995000000000001</v>
+        <v>20.430099999999999</v>
       </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.2">
@@ -16484,7 +16526,7 @@
         <v>#N/A</v>
       </c>
       <c r="F264">
-        <v>19.2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.2">
@@ -16507,7 +16549,7 @@
         <v>#N/A</v>
       </c>
       <c r="F265">
-        <v>25.17</v>
+        <v>24.75</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.2">
@@ -16530,7 +16572,7 @@
         <v>#N/A</v>
       </c>
       <c r="F266">
-        <v>23.23</v>
+        <v>22.91</v>
       </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.2">
@@ -16553,7 +16595,7 @@
         <v>#N/A</v>
       </c>
       <c r="F267">
-        <v>23.25</v>
+        <v>23.15</v>
       </c>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.2">
@@ -16576,7 +16618,7 @@
         <v>#N/A</v>
       </c>
       <c r="F268">
-        <v>21.73</v>
+        <v>20.170000000000002</v>
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.2">
@@ -16599,7 +16641,7 @@
         <v>#N/A</v>
       </c>
       <c r="F269">
-        <v>21.72</v>
+        <v>20.260000000000002</v>
       </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.2">
@@ -16714,7 +16756,7 @@
         <v>#N/A</v>
       </c>
       <c r="F274">
-        <v>47.580100000000002</v>
+        <v>46.95</v>
       </c>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.2">
@@ -16737,7 +16779,7 @@
         <v>#N/A</v>
       </c>
       <c r="F275">
-        <v>23.650099999999998</v>
+        <v>22.35</v>
       </c>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.2">
@@ -16760,7 +16802,7 @@
         <v>#N/A</v>
       </c>
       <c r="F276">
-        <v>25.38</v>
+        <v>25.19</v>
       </c>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.2">
@@ -16783,7 +16825,7 @@
         <v>#N/A</v>
       </c>
       <c r="F277">
-        <v>23.64</v>
+        <v>23.58</v>
       </c>
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.2">
@@ -16806,7 +16848,7 @@
         <v>#N/A</v>
       </c>
       <c r="F278">
-        <v>24.73</v>
+        <v>24.51</v>
       </c>
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.2">
@@ -16829,7 +16871,7 @@
         <v>#N/A</v>
       </c>
       <c r="F279">
-        <v>21.52</v>
+        <v>21</v>
       </c>
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.2">
@@ -16852,7 +16894,7 @@
         <v>#N/A</v>
       </c>
       <c r="F280">
-        <v>19.73</v>
+        <v>18.670000000000002</v>
       </c>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.2">
@@ -16875,7 +16917,7 @@
         <v>#N/A</v>
       </c>
       <c r="F281">
-        <v>19.690000000000001</v>
+        <v>19.149999999999999</v>
       </c>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.2">
@@ -17013,7 +17055,7 @@
         <v>#N/A</v>
       </c>
       <c r="F287">
-        <v>17.489999999999998</v>
+        <v>17.100000000000001</v>
       </c>
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.2">
@@ -17036,7 +17078,7 @@
         <v>#N/A</v>
       </c>
       <c r="F288">
-        <v>19</v>
+        <v>18.850000000000001</v>
       </c>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.2">
@@ -17059,7 +17101,7 @@
         <v>#N/A</v>
       </c>
       <c r="F289">
-        <v>17.079999999999998</v>
+        <v>16.8</v>
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.2">
@@ -17082,7 +17124,7 @@
         <v>#N/A</v>
       </c>
       <c r="F290">
-        <v>18.670000000000002</v>
+        <v>17.850000000000001</v>
       </c>
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.2">
@@ -17128,7 +17170,7 @@
         <v>#N/A</v>
       </c>
       <c r="F292">
-        <v>21.26</v>
+        <v>21.1</v>
       </c>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.2">
@@ -17151,7 +17193,7 @@
         <v>#N/A</v>
       </c>
       <c r="F293">
-        <v>25.54</v>
+        <v>25.53</v>
       </c>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.2">
@@ -17174,7 +17216,7 @@
         <v>#N/A</v>
       </c>
       <c r="F294">
-        <v>25.34</v>
+        <v>25.4</v>
       </c>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.2">
@@ -17197,7 +17239,7 @@
         <v>#N/A</v>
       </c>
       <c r="F295">
-        <v>25.34</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.2">
@@ -17220,7 +17262,7 @@
         <v>#N/A</v>
       </c>
       <c r="F296">
-        <v>24.95</v>
+        <v>24.33</v>
       </c>
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.2">
@@ -17243,7 +17285,7 @@
         <v>#N/A</v>
       </c>
       <c r="F297">
-        <v>21.75</v>
+        <v>21.43</v>
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.2">
@@ -17266,7 +17308,7 @@
         <v>#N/A</v>
       </c>
       <c r="F298">
-        <v>73.2</v>
+        <v>71.91</v>
       </c>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.2">
@@ -17381,7 +17423,7 @@
         <v>#N/A</v>
       </c>
       <c r="F303">
-        <v>24.963899999999999</v>
+        <v>24.35</v>
       </c>
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.2">
@@ -17519,7 +17561,7 @@
         <v>#N/A</v>
       </c>
       <c r="F309">
-        <v>23.27</v>
+        <v>24.26</v>
       </c>
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.2">
@@ -17565,7 +17607,7 @@
         <v>#N/A</v>
       </c>
       <c r="F311">
-        <v>25.04</v>
+        <v>23.97</v>
       </c>
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.2">
@@ -17611,7 +17653,7 @@
         <v>#N/A</v>
       </c>
       <c r="F313">
-        <v>25.04</v>
+        <v>24.46</v>
       </c>
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.2">
@@ -17634,7 +17676,7 @@
         <v>#N/A</v>
       </c>
       <c r="F314">
-        <v>24.28</v>
+        <v>23.35</v>
       </c>
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.2">
@@ -17657,7 +17699,7 @@
         <v>#N/A</v>
       </c>
       <c r="F315">
-        <v>24.04</v>
+        <v>23.51</v>
       </c>
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.2">
@@ -17703,7 +17745,7 @@
         <v>#N/A</v>
       </c>
       <c r="F317">
-        <v>23.53</v>
+        <v>23.26</v>
       </c>
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.2">
@@ -17726,7 +17768,7 @@
         <v>#N/A</v>
       </c>
       <c r="F318">
-        <v>23.46</v>
+        <v>22.83</v>
       </c>
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.2">
@@ -17749,7 +17791,7 @@
         <v>#N/A</v>
       </c>
       <c r="F319">
-        <v>22.7</v>
+        <v>22.24</v>
       </c>
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.2">
@@ -17772,7 +17814,7 @@
         <v>#N/A</v>
       </c>
       <c r="F320">
-        <v>20.09</v>
+        <v>19.47</v>
       </c>
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.2">
@@ -17795,7 +17837,7 @@
         <v>#N/A</v>
       </c>
       <c r="F321">
-        <v>25.204999999999998</v>
+        <v>24.91</v>
       </c>
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.2">
@@ -17818,7 +17860,7 @@
         <v>#N/A</v>
       </c>
       <c r="F322">
-        <v>23.76</v>
+        <v>23.59</v>
       </c>
     </row>
     <row r="323" spans="1:6" x14ac:dyDescent="0.2">
@@ -17841,7 +17883,7 @@
         <v>#N/A</v>
       </c>
       <c r="F323">
-        <v>25.15</v>
+        <v>25.21</v>
       </c>
     </row>
     <row r="324" spans="1:6" x14ac:dyDescent="0.2">
@@ -17864,7 +17906,7 @@
         <v>#N/A</v>
       </c>
       <c r="F324">
-        <v>23.71</v>
+        <v>23.3</v>
       </c>
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.2">
@@ -17887,7 +17929,7 @@
         <v>#N/A</v>
       </c>
       <c r="F325">
-        <v>25.8</v>
+        <v>25.86</v>
       </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.2">
@@ -17910,7 +17952,7 @@
         <v>#N/A</v>
       </c>
       <c r="F326">
-        <v>21.38</v>
+        <v>21.1</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.2">
@@ -17933,7 +17975,7 @@
         <v>#N/A</v>
       </c>
       <c r="F327">
-        <v>24.75</v>
+        <v>22.43</v>
       </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.2">
@@ -17956,7 +17998,7 @@
         <v>#N/A</v>
       </c>
       <c r="F328">
-        <v>43.875</v>
+        <v>41.645000000000003</v>
       </c>
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.2">
@@ -17979,7 +18021,7 @@
         <v>#N/A</v>
       </c>
       <c r="F329">
-        <v>22.8</v>
+        <v>21.8</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.2">
@@ -18002,7 +18044,7 @@
         <v>#N/A</v>
       </c>
       <c r="F330">
-        <v>20.45</v>
+        <v>19.489999999999998</v>
       </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.2">
@@ -18025,7 +18067,7 @@
         <v>#N/A</v>
       </c>
       <c r="F331">
-        <v>23.47</v>
+        <v>23.11</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.2">
@@ -18048,7 +18090,7 @@
         <v>#N/A</v>
       </c>
       <c r="F332">
-        <v>23.53</v>
+        <v>22.84</v>
       </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.2">
@@ -18094,7 +18136,7 @@
         <v>#N/A</v>
       </c>
       <c r="F334">
-        <v>19.600000000000001</v>
+        <v>18.2</v>
       </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.2">
@@ -18163,7 +18205,7 @@
         <v>#N/A</v>
       </c>
       <c r="F337">
-        <v>18.13</v>
+        <v>17.670000000000002</v>
       </c>
     </row>
     <row r="338" spans="1:6" x14ac:dyDescent="0.2">
@@ -18186,7 +18228,7 @@
         <v>#N/A</v>
       </c>
       <c r="F338">
-        <v>22.1</v>
+        <v>21.72</v>
       </c>
     </row>
     <row r="339" spans="1:6" x14ac:dyDescent="0.2">
@@ -18255,7 +18297,7 @@
         <v>#N/A</v>
       </c>
       <c r="F341">
-        <v>20.84</v>
+        <v>19.559999999999999</v>
       </c>
     </row>
     <row r="342" spans="1:6" x14ac:dyDescent="0.2">
@@ -18278,7 +18320,7 @@
         <v>#N/A</v>
       </c>
       <c r="F342">
-        <v>20.62</v>
+        <v>19.510000000000002</v>
       </c>
     </row>
     <row r="343" spans="1:6" x14ac:dyDescent="0.2">
@@ -18370,7 +18412,7 @@
         <v>#N/A</v>
       </c>
       <c r="F346">
-        <v>24.07</v>
+        <v>23.734999999999999</v>
       </c>
     </row>
     <row r="347" spans="1:6" x14ac:dyDescent="0.2">
@@ -18393,7 +18435,7 @@
         <v>#N/A</v>
       </c>
       <c r="F347">
-        <v>23.36</v>
+        <v>22.8</v>
       </c>
     </row>
     <row r="348" spans="1:6" x14ac:dyDescent="0.2">
@@ -18462,7 +18504,7 @@
         <v>#N/A</v>
       </c>
       <c r="F350">
-        <v>25.43</v>
+        <v>24.08</v>
       </c>
     </row>
     <row r="351" spans="1:6" x14ac:dyDescent="0.2">
@@ -18577,7 +18619,7 @@
         <v>#N/A</v>
       </c>
       <c r="F355">
-        <v>25.14</v>
+        <v>24.91</v>
       </c>
     </row>
     <row r="356" spans="1:6" x14ac:dyDescent="0.2">
@@ -18600,7 +18642,7 @@
         <v>#N/A</v>
       </c>
       <c r="F356">
-        <v>24.78</v>
+        <v>24.42</v>
       </c>
     </row>
     <row r="357" spans="1:6" x14ac:dyDescent="0.2">
@@ -18715,7 +18757,7 @@
         <v>#N/A</v>
       </c>
       <c r="F361">
-        <v>23.12</v>
+        <v>22.712800000000001</v>
       </c>
     </row>
     <row r="362" spans="1:6" x14ac:dyDescent="0.2">
@@ -18738,7 +18780,7 @@
         <v>#N/A</v>
       </c>
       <c r="F362">
-        <v>23.07</v>
+        <v>22.27</v>
       </c>
     </row>
     <row r="363" spans="1:6" x14ac:dyDescent="0.2">
@@ -18761,7 +18803,7 @@
         <v>#N/A</v>
       </c>
       <c r="F363">
-        <v>24.8</v>
+        <v>24.32</v>
       </c>
     </row>
     <row r="364" spans="1:6" x14ac:dyDescent="0.2">
@@ -18784,7 +18826,7 @@
         <v>#N/A</v>
       </c>
       <c r="F364">
-        <v>21.7</v>
+        <v>20.94</v>
       </c>
     </row>
     <row r="365" spans="1:6" x14ac:dyDescent="0.2">
@@ -18807,7 +18849,7 @@
         <v>#N/A</v>
       </c>
       <c r="F365">
-        <v>21.11</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="366" spans="1:6" x14ac:dyDescent="0.2">
@@ -18830,7 +18872,7 @@
         <v>#N/A</v>
       </c>
       <c r="F366">
-        <v>21.04</v>
+        <v>20.52</v>
       </c>
     </row>
     <row r="367" spans="1:6" x14ac:dyDescent="0.2">
@@ -18853,7 +18895,7 @@
         <v>#N/A</v>
       </c>
       <c r="F367">
-        <v>20.43</v>
+        <v>19.98</v>
       </c>
     </row>
     <row r="368" spans="1:6" x14ac:dyDescent="0.2">
@@ -19129,7 +19171,7 @@
         <v>#N/A</v>
       </c>
       <c r="F379">
-        <v>13.75</v>
+        <v>12.14</v>
       </c>
     </row>
     <row r="380" spans="1:6" x14ac:dyDescent="0.2">
@@ -19152,7 +19194,7 @@
         <v>#N/A</v>
       </c>
       <c r="F380">
-        <v>14.299899999999999</v>
+        <v>12.26</v>
       </c>
     </row>
     <row r="381" spans="1:6" x14ac:dyDescent="0.2">
@@ -19198,7 +19240,7 @@
         <v>#N/A</v>
       </c>
       <c r="F382">
-        <v>23.52</v>
+        <v>23.15</v>
       </c>
     </row>
     <row r="383" spans="1:6" x14ac:dyDescent="0.2">
@@ -19244,7 +19286,7 @@
         <v>#N/A</v>
       </c>
       <c r="F384">
-        <v>25.58</v>
+        <v>25.09</v>
       </c>
     </row>
     <row r="385" spans="1:6" x14ac:dyDescent="0.2">
@@ -19267,7 +19309,7 @@
         <v>#N/A</v>
       </c>
       <c r="F385">
-        <v>24.28</v>
+        <v>22.08</v>
       </c>
     </row>
     <row r="386" spans="1:6" x14ac:dyDescent="0.2">
@@ -19290,7 +19332,7 @@
         <v>#N/A</v>
       </c>
       <c r="F386">
-        <v>20.89</v>
+        <v>20</v>
       </c>
     </row>
     <row r="387" spans="1:6" x14ac:dyDescent="0.2">
@@ -19359,7 +19401,7 @@
         <v>#N/A</v>
       </c>
       <c r="F389">
-        <v>23.33</v>
+        <v>22.65</v>
       </c>
     </row>
     <row r="390" spans="1:6" x14ac:dyDescent="0.2">
@@ -19382,7 +19424,7 @@
         <v>#N/A</v>
       </c>
       <c r="F390">
-        <v>21.99</v>
+        <v>21.12</v>
       </c>
     </row>
     <row r="391" spans="1:6" x14ac:dyDescent="0.2">
@@ -19405,7 +19447,7 @@
         <v>#N/A</v>
       </c>
       <c r="F391">
-        <v>24.2</v>
+        <v>24.23</v>
       </c>
     </row>
     <row r="392" spans="1:6" x14ac:dyDescent="0.2">
@@ -19428,7 +19470,7 @@
         <v>#N/A</v>
       </c>
       <c r="F392">
-        <v>18.649999999999999</v>
+        <v>17.98</v>
       </c>
     </row>
     <row r="393" spans="1:6" x14ac:dyDescent="0.2">
@@ -19451,7 +19493,7 @@
         <v>#N/A</v>
       </c>
       <c r="F393">
-        <v>24.75</v>
+        <v>24.414999999999999</v>
       </c>
     </row>
     <row r="394" spans="1:6" x14ac:dyDescent="0.2">
@@ -19497,7 +19539,7 @@
         <v>#N/A</v>
       </c>
       <c r="F395">
-        <v>23.15</v>
+        <v>22.765000000000001</v>
       </c>
     </row>
     <row r="396" spans="1:6" x14ac:dyDescent="0.2">
@@ -19543,7 +19585,7 @@
         <v>#N/A</v>
       </c>
       <c r="F397">
-        <v>25.45</v>
+        <v>25.06</v>
       </c>
     </row>
     <row r="398" spans="1:6" x14ac:dyDescent="0.2">
@@ -19589,7 +19631,7 @@
         <v>#N/A</v>
       </c>
       <c r="F399">
-        <v>20.47</v>
+        <v>20.380400000000002</v>
       </c>
     </row>
     <row r="400" spans="1:6" x14ac:dyDescent="0.2">
@@ -19612,7 +19654,7 @@
         <v>#N/A</v>
       </c>
       <c r="F400">
-        <v>23.21</v>
+        <v>22.29</v>
       </c>
     </row>
     <row r="401" spans="1:6" x14ac:dyDescent="0.2">
@@ -19635,7 +19677,7 @@
         <v>#N/A</v>
       </c>
       <c r="F401">
-        <v>19.967099999999999</v>
+        <v>20.54</v>
       </c>
     </row>
     <row r="402" spans="1:6" x14ac:dyDescent="0.2">
@@ -19658,7 +19700,7 @@
         <v>#N/A</v>
       </c>
       <c r="F402">
-        <v>22.649699999999999</v>
+        <v>23.18</v>
       </c>
     </row>
     <row r="403" spans="1:6" x14ac:dyDescent="0.2">
@@ -19681,7 +19723,7 @@
         <v>#N/A</v>
       </c>
       <c r="F403">
-        <v>19.940000000000001</v>
+        <v>19.989999999999998</v>
       </c>
     </row>
     <row r="404" spans="1:6" x14ac:dyDescent="0.2">
@@ -19727,7 +19769,7 @@
         <v>#N/A</v>
       </c>
       <c r="F405">
-        <v>24.900600000000001</v>
+        <v>24.39</v>
       </c>
     </row>
     <row r="406" spans="1:6" x14ac:dyDescent="0.2">
@@ -19773,7 +19815,7 @@
         <v>#N/A</v>
       </c>
       <c r="F407">
-        <v>24.85</v>
+        <v>24.35</v>
       </c>
     </row>
     <row r="408" spans="1:6" x14ac:dyDescent="0.2">
@@ -19796,7 +19838,7 @@
         <v>#N/A</v>
       </c>
       <c r="F408">
-        <v>24.73</v>
+        <v>24.14</v>
       </c>
     </row>
     <row r="409" spans="1:6" x14ac:dyDescent="0.2">
@@ -19819,7 +19861,7 @@
         <v>#N/A</v>
       </c>
       <c r="F409">
-        <v>22</v>
+        <v>20.95</v>
       </c>
     </row>
     <row r="410" spans="1:6" x14ac:dyDescent="0.2">
@@ -19865,7 +19907,7 @@
         <v>#N/A</v>
       </c>
       <c r="F411">
-        <v>24.12</v>
+        <v>23.76</v>
       </c>
     </row>
     <row r="412" spans="1:6" x14ac:dyDescent="0.2">
@@ -19911,7 +19953,7 @@
         <v>#N/A</v>
       </c>
       <c r="F413">
-        <v>20.23</v>
+        <v>15.23</v>
       </c>
     </row>
     <row r="414" spans="1:6" x14ac:dyDescent="0.2">
@@ -19934,7 +19976,7 @@
         <v>#N/A</v>
       </c>
       <c r="F414" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="415" spans="1:6" x14ac:dyDescent="0.2">
@@ -19980,7 +20022,7 @@
         <v>#N/A</v>
       </c>
       <c r="F416">
-        <v>22.32</v>
+        <v>21.07</v>
       </c>
     </row>
     <row r="417" spans="1:6" x14ac:dyDescent="0.2">
@@ -20003,7 +20045,7 @@
         <v>#N/A</v>
       </c>
       <c r="F417">
-        <v>63.120927500000001</v>
+        <v>66.22</v>
       </c>
     </row>
     <row r="418" spans="1:6" x14ac:dyDescent="0.2">
@@ -20026,7 +20068,7 @@
         <v>#N/A</v>
       </c>
       <c r="F418">
-        <v>24.95</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="419" spans="1:6" x14ac:dyDescent="0.2">
@@ -20049,7 +20091,7 @@
         <v>#N/A</v>
       </c>
       <c r="F419">
-        <v>24.52</v>
+        <v>24.02</v>
       </c>
     </row>
     <row r="420" spans="1:6" x14ac:dyDescent="0.2">
@@ -20118,7 +20160,7 @@
         <v>#N/A</v>
       </c>
       <c r="F422">
-        <v>23.83</v>
+        <v>23.38</v>
       </c>
     </row>
     <row r="423" spans="1:6" x14ac:dyDescent="0.2">
@@ -20141,7 +20183,7 @@
         <v>#N/A</v>
       </c>
       <c r="F423">
-        <v>21.7</v>
+        <v>21.15</v>
       </c>
     </row>
     <row r="424" spans="1:6" x14ac:dyDescent="0.2">
@@ -20187,7 +20229,7 @@
         <v>#N/A</v>
       </c>
       <c r="F425">
-        <v>23.08</v>
+        <v>23.02</v>
       </c>
     </row>
     <row r="426" spans="1:6" x14ac:dyDescent="0.2">
@@ -20210,7 +20252,7 @@
         <v>#N/A</v>
       </c>
       <c r="F426">
-        <v>24.51</v>
+        <v>23.69</v>
       </c>
     </row>
     <row r="427" spans="1:6" x14ac:dyDescent="0.2">
@@ -20233,7 +20275,7 @@
         <v>#N/A</v>
       </c>
       <c r="F427">
-        <v>23.8</v>
+        <v>23.6723</v>
       </c>
     </row>
     <row r="428" spans="1:6" x14ac:dyDescent="0.2">
@@ -20302,7 +20344,7 @@
         <v>#N/A</v>
       </c>
       <c r="F430">
-        <v>23.96</v>
+        <v>23.76</v>
       </c>
     </row>
     <row r="431" spans="1:6" x14ac:dyDescent="0.2">
@@ -20325,7 +20367,7 @@
         <v>#N/A</v>
       </c>
       <c r="F431">
-        <v>24.87</v>
+        <v>24.88</v>
       </c>
     </row>
     <row r="432" spans="1:6" x14ac:dyDescent="0.2">
@@ -20348,7 +20390,7 @@
         <v>#N/A</v>
       </c>
       <c r="F432">
-        <v>24.83</v>
+        <v>24.728100000000001</v>
       </c>
     </row>
     <row r="433" spans="1:6" x14ac:dyDescent="0.2">
@@ -20394,7 +20436,7 @@
         <v>#N/A</v>
       </c>
       <c r="F434">
-        <v>24.91</v>
+        <v>24.37</v>
       </c>
     </row>
     <row r="435" spans="1:6" x14ac:dyDescent="0.2">
@@ -20417,7 +20459,7 @@
         <v>#N/A</v>
       </c>
       <c r="F435">
-        <v>24.83</v>
+        <v>24.37</v>
       </c>
     </row>
     <row r="436" spans="1:6" x14ac:dyDescent="0.2">
@@ -20463,7 +20505,7 @@
         <v>#N/A</v>
       </c>
       <c r="F437">
-        <v>18.8</v>
+        <v>18.03</v>
       </c>
     </row>
     <row r="438" spans="1:6" x14ac:dyDescent="0.2">
@@ -20486,7 +20528,7 @@
         <v>#N/A</v>
       </c>
       <c r="F438">
-        <v>20.97</v>
+        <v>20.29</v>
       </c>
     </row>
     <row r="439" spans="1:6" x14ac:dyDescent="0.2">
@@ -20509,7 +20551,7 @@
         <v>#N/A</v>
       </c>
       <c r="F439">
-        <v>19.75</v>
+        <v>19.149999999999999</v>
       </c>
     </row>
     <row r="440" spans="1:6" x14ac:dyDescent="0.2">
@@ -20532,7 +20574,7 @@
         <v>#N/A</v>
       </c>
       <c r="F440">
-        <v>25.33</v>
+        <v>25.46</v>
       </c>
     </row>
     <row r="441" spans="1:6" x14ac:dyDescent="0.2">
@@ -20555,7 +20597,7 @@
         <v>#N/A</v>
       </c>
       <c r="F441">
-        <v>25.19</v>
+        <v>25.26</v>
       </c>
     </row>
     <row r="442" spans="1:6" x14ac:dyDescent="0.2">
@@ -20578,7 +20620,7 @@
         <v>#N/A</v>
       </c>
       <c r="F442">
-        <v>25.34</v>
+        <v>25.46</v>
       </c>
     </row>
     <row r="443" spans="1:6" x14ac:dyDescent="0.2">
@@ -20601,7 +20643,7 @@
         <v>#N/A</v>
       </c>
       <c r="F443">
-        <v>23.32</v>
+        <v>22.83</v>
       </c>
     </row>
     <row r="444" spans="1:6" x14ac:dyDescent="0.2">
@@ -20624,7 +20666,7 @@
         <v>#N/A</v>
       </c>
       <c r="F444">
-        <v>24.75</v>
+        <v>24.17</v>
       </c>
     </row>
     <row r="445" spans="1:6" x14ac:dyDescent="0.2">
@@ -20900,7 +20942,7 @@
         <v>#N/A</v>
       </c>
       <c r="F456">
-        <v>21.94</v>
+        <v>21.33</v>
       </c>
     </row>
     <row r="457" spans="1:6" x14ac:dyDescent="0.2">
@@ -20923,7 +20965,7 @@
         <v>#N/A</v>
       </c>
       <c r="F457">
-        <v>23.22</v>
+        <v>22.6</v>
       </c>
     </row>
     <row r="458" spans="1:6" x14ac:dyDescent="0.2">
@@ -20946,7 +20988,7 @@
         <v>#N/A</v>
       </c>
       <c r="F458">
-        <v>24.45</v>
+        <v>24.467400000000001</v>
       </c>
     </row>
     <row r="459" spans="1:6" x14ac:dyDescent="0.2">
@@ -20969,7 +21011,7 @@
         <v>#N/A</v>
       </c>
       <c r="F459">
-        <v>24.03</v>
+        <v>24</v>
       </c>
     </row>
     <row r="460" spans="1:6" x14ac:dyDescent="0.2">
@@ -21015,7 +21057,7 @@
         <v>#N/A</v>
       </c>
       <c r="F461">
-        <v>25.61</v>
+        <v>24.94</v>
       </c>
     </row>
     <row r="462" spans="1:6" x14ac:dyDescent="0.2">
@@ -21038,7 +21080,7 @@
         <v>#N/A</v>
       </c>
       <c r="F462">
-        <v>24.752500000000001</v>
+        <v>24.44</v>
       </c>
     </row>
     <row r="463" spans="1:6" x14ac:dyDescent="0.2">
@@ -21061,7 +21103,7 @@
         <v>#N/A</v>
       </c>
       <c r="F463">
-        <v>24.55</v>
+        <v>23.549299999999999</v>
       </c>
     </row>
     <row r="464" spans="1:6" x14ac:dyDescent="0.2">
@@ -21084,7 +21126,7 @@
         <v>#N/A</v>
       </c>
       <c r="F464">
-        <v>21.39</v>
+        <v>21.12</v>
       </c>
     </row>
     <row r="465" spans="1:6" x14ac:dyDescent="0.2">
@@ -21107,7 +21149,7 @@
         <v>#N/A</v>
       </c>
       <c r="F465">
-        <v>21.17</v>
+        <v>20.95</v>
       </c>
     </row>
     <row r="466" spans="1:6" x14ac:dyDescent="0.2">
@@ -21130,7 +21172,7 @@
         <v>#N/A</v>
       </c>
       <c r="F466">
-        <v>22.12</v>
+        <v>21.4</v>
       </c>
     </row>
     <row r="467" spans="1:6" x14ac:dyDescent="0.2">
@@ -21153,7 +21195,7 @@
         <v>#N/A</v>
       </c>
       <c r="F467">
-        <v>21.12</v>
+        <v>20.55</v>
       </c>
     </row>
     <row r="468" spans="1:6" x14ac:dyDescent="0.2">
@@ -21176,7 +21218,7 @@
         <v>#N/A</v>
       </c>
       <c r="F468">
-        <v>21.35</v>
+        <v>21.2</v>
       </c>
     </row>
     <row r="469" spans="1:6" x14ac:dyDescent="0.2">
@@ -21222,7 +21264,7 @@
         <v>#N/A</v>
       </c>
       <c r="F470">
-        <v>21.6</v>
+        <v>21.9</v>
       </c>
     </row>
     <row r="471" spans="1:6" x14ac:dyDescent="0.2">
@@ -21245,7 +21287,7 @@
         <v>#N/A</v>
       </c>
       <c r="F471">
-        <v>20.39</v>
+        <v>20.85</v>
       </c>
     </row>
     <row r="472" spans="1:6" x14ac:dyDescent="0.2">
@@ -21291,7 +21333,7 @@
         <v>#N/A</v>
       </c>
       <c r="F473">
-        <v>22.39</v>
+        <v>21.88</v>
       </c>
     </row>
     <row r="474" spans="1:6" x14ac:dyDescent="0.2">
@@ -21314,7 +21356,7 @@
         <v>#N/A</v>
       </c>
       <c r="F474">
-        <v>23.9664</v>
+        <v>23.45</v>
       </c>
     </row>
     <row r="475" spans="1:6" x14ac:dyDescent="0.2">
@@ -21337,7 +21379,7 @@
         <v>#N/A</v>
       </c>
       <c r="F475">
-        <v>20.85</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="476" spans="1:6" x14ac:dyDescent="0.2">
@@ -21406,7 +21448,7 @@
         <v>#N/A</v>
       </c>
       <c r="F478">
-        <v>24.41</v>
+        <v>23.91</v>
       </c>
     </row>
     <row r="479" spans="1:6" x14ac:dyDescent="0.2">
@@ -21429,7 +21471,7 @@
         <v>#N/A</v>
       </c>
       <c r="F479">
-        <v>23.21</v>
+        <v>23.86</v>
       </c>
     </row>
     <row r="480" spans="1:6" x14ac:dyDescent="0.2">
@@ -21544,7 +21586,7 @@
         <v>#N/A</v>
       </c>
       <c r="F484">
-        <v>25.44</v>
+        <v>25.27</v>
       </c>
     </row>
     <row r="485" spans="1:6" x14ac:dyDescent="0.2">
@@ -21567,7 +21609,7 @@
         <v>#N/A</v>
       </c>
       <c r="F485">
-        <v>25</v>
+        <v>24.91</v>
       </c>
     </row>
     <row r="486" spans="1:6" x14ac:dyDescent="0.2">
@@ -21613,7 +21655,7 @@
         <v>#N/A</v>
       </c>
       <c r="F487">
-        <v>16.855</v>
+        <v>15.6</v>
       </c>
     </row>
     <row r="488" spans="1:6" x14ac:dyDescent="0.2">
@@ -21636,7 +21678,7 @@
         <v>#N/A</v>
       </c>
       <c r="F488">
-        <v>16.190000000000001</v>
+        <v>15.38</v>
       </c>
     </row>
     <row r="489" spans="1:6" x14ac:dyDescent="0.2">
@@ -21659,7 +21701,7 @@
         <v>#N/A</v>
       </c>
       <c r="F489">
-        <v>23.78</v>
+        <v>23.48</v>
       </c>
     </row>
     <row r="490" spans="1:6" x14ac:dyDescent="0.2">
@@ -21728,7 +21770,7 @@
         <v>#N/A</v>
       </c>
       <c r="F492">
-        <v>27.46</v>
+        <v>27.489599999999999</v>
       </c>
     </row>
     <row r="493" spans="1:6" x14ac:dyDescent="0.2">
@@ -21751,7 +21793,7 @@
         <v>#N/A</v>
       </c>
       <c r="F493">
-        <v>1181</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="494" spans="1:6" x14ac:dyDescent="0.2">
@@ -21843,7 +21885,7 @@
         <v>#N/A</v>
       </c>
       <c r="F497">
-        <v>24.65</v>
+        <v>24.47</v>
       </c>
     </row>
     <row r="498" spans="1:6" x14ac:dyDescent="0.2">
@@ -21866,7 +21908,7 @@
         <v>#N/A</v>
       </c>
       <c r="F498">
-        <v>25.15</v>
+        <v>24.77</v>
       </c>
     </row>
     <row r="499" spans="1:6" x14ac:dyDescent="0.2">
@@ -21981,7 +22023,7 @@
         <v>#N/A</v>
       </c>
       <c r="F503">
-        <v>23.7239</v>
+        <v>22.84</v>
       </c>
     </row>
     <row r="504" spans="1:6" x14ac:dyDescent="0.2">
@@ -22004,7 +22046,7 @@
         <v>#N/A</v>
       </c>
       <c r="F504">
-        <v>19.760000000000002</v>
+        <v>18.95</v>
       </c>
     </row>
     <row r="505" spans="1:6" x14ac:dyDescent="0.2">
@@ -22119,7 +22161,7 @@
         <v>#N/A</v>
       </c>
       <c r="F509">
-        <v>23.78</v>
+        <v>23.600100000000001</v>
       </c>
     </row>
     <row r="510" spans="1:6" x14ac:dyDescent="0.2">
@@ -22142,7 +22184,7 @@
         <v>#N/A</v>
       </c>
       <c r="F510">
-        <v>22.15</v>
+        <v>21.77</v>
       </c>
     </row>
     <row r="511" spans="1:6" x14ac:dyDescent="0.2">
@@ -22165,7 +22207,7 @@
         <v>#N/A</v>
       </c>
       <c r="F511">
-        <v>25.336200000000002</v>
+        <v>25.0212</v>
       </c>
     </row>
     <row r="512" spans="1:6" x14ac:dyDescent="0.2">
@@ -22188,7 +22230,7 @@
         <v>#N/A</v>
       </c>
       <c r="F512">
-        <v>25.51</v>
+        <v>24.96</v>
       </c>
     </row>
     <row r="513" spans="1:6" x14ac:dyDescent="0.2">
@@ -22234,7 +22276,7 @@
         <v>#N/A</v>
       </c>
       <c r="F514">
-        <v>25.14</v>
+        <v>24.15</v>
       </c>
     </row>
     <row r="515" spans="1:6" x14ac:dyDescent="0.2">
@@ -22257,7 +22299,7 @@
         <v>#N/A</v>
       </c>
       <c r="F515">
-        <v>137.34</v>
+        <v>141.44</v>
       </c>
     </row>
     <row r="516" spans="1:6" x14ac:dyDescent="0.2">
@@ -22280,7 +22322,7 @@
         <v>#N/A</v>
       </c>
       <c r="F516">
-        <v>23.905000000000001</v>
+        <v>23.886199999999999</v>
       </c>
     </row>
     <row r="517" spans="1:6" x14ac:dyDescent="0.2">
@@ -22303,7 +22345,7 @@
         <v>#N/A</v>
       </c>
       <c r="F517">
-        <v>25.87</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="518" spans="1:6" x14ac:dyDescent="0.2">
@@ -22326,7 +22368,7 @@
         <v>#N/A</v>
       </c>
       <c r="F518">
-        <v>21.76</v>
+        <v>21.1</v>
       </c>
     </row>
     <row r="519" spans="1:6" x14ac:dyDescent="0.2">
@@ -22349,7 +22391,7 @@
         <v>#N/A</v>
       </c>
       <c r="F519">
-        <v>20.73</v>
+        <v>20.07</v>
       </c>
     </row>
     <row r="520" spans="1:6" x14ac:dyDescent="0.2">
@@ -22372,7 +22414,7 @@
         <v>#N/A</v>
       </c>
       <c r="F520">
-        <v>66.87</v>
+        <v>65.27</v>
       </c>
     </row>
     <row r="521" spans="1:6" x14ac:dyDescent="0.2">
@@ -22395,7 +22437,7 @@
         <v>#N/A</v>
       </c>
       <c r="F521">
-        <v>48.715000000000003</v>
+        <v>49.44</v>
       </c>
     </row>
     <row r="522" spans="1:6" x14ac:dyDescent="0.2">
@@ -22418,7 +22460,7 @@
         <v>#N/A</v>
       </c>
       <c r="F522">
-        <v>190.68</v>
+        <v>182.29</v>
       </c>
     </row>
     <row r="523" spans="1:6" x14ac:dyDescent="0.2">
@@ -22441,7 +22483,7 @@
         <v>#N/A</v>
       </c>
       <c r="F523">
-        <v>18</v>
+        <v>18.149999999999999</v>
       </c>
     </row>
     <row r="524" spans="1:6" x14ac:dyDescent="0.2">
@@ -22464,7 +22506,7 @@
         <v>#N/A</v>
       </c>
       <c r="F524">
-        <v>18.39</v>
+        <v>17.690000000000001</v>
       </c>
     </row>
     <row r="525" spans="1:6" x14ac:dyDescent="0.2">
@@ -22487,7 +22529,7 @@
         <v>#N/A</v>
       </c>
       <c r="F525">
-        <v>25.64</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="526" spans="1:6" x14ac:dyDescent="0.2">
@@ -22533,7 +22575,7 @@
         <v>#N/A</v>
       </c>
       <c r="F527">
-        <v>45.87</v>
+        <v>47.23</v>
       </c>
     </row>
     <row r="528" spans="1:6" x14ac:dyDescent="0.2">
@@ -22556,7 +22598,7 @@
         <v>#N/A</v>
       </c>
       <c r="F528">
-        <v>43.85</v>
+        <v>40.53</v>
       </c>
     </row>
     <row r="529" spans="1:6" x14ac:dyDescent="0.2">
@@ -22579,7 +22621,7 @@
         <v>#N/A</v>
       </c>
       <c r="F529">
-        <v>828.45</v>
+        <v>820</v>
       </c>
     </row>
     <row r="530" spans="1:6" x14ac:dyDescent="0.2">
@@ -22602,7 +22644,7 @@
         <v>#N/A</v>
       </c>
       <c r="F530">
-        <v>19.329999999999998</v>
+        <v>19.079999999999998</v>
       </c>
     </row>
     <row r="531" spans="1:6" x14ac:dyDescent="0.2">
@@ -22625,7 +22667,7 @@
         <v>#N/A</v>
       </c>
       <c r="F531">
-        <v>19.399999999999999</v>
+        <v>18.93</v>
       </c>
     </row>
     <row r="532" spans="1:6" x14ac:dyDescent="0.2">
@@ -22648,7 +22690,7 @@
         <v>#N/A</v>
       </c>
       <c r="F532">
-        <v>17.510000000000002</v>
+        <v>16.45</v>
       </c>
     </row>
     <row r="533" spans="1:6" x14ac:dyDescent="0.2">
@@ -22671,7 +22713,7 @@
         <v>#N/A</v>
       </c>
       <c r="F533">
-        <v>69.838200000000001</v>
+        <v>66.52</v>
       </c>
     </row>
     <row r="534" spans="1:6" x14ac:dyDescent="0.2">
@@ -22694,7 +22736,7 @@
         <v>#N/A</v>
       </c>
       <c r="F534">
-        <v>19.36</v>
+        <v>19.18</v>
       </c>
     </row>
     <row r="535" spans="1:6" x14ac:dyDescent="0.2">
@@ -22717,7 +22759,7 @@
         <v>#N/A</v>
       </c>
       <c r="F535">
-        <v>19.260000000000002</v>
+        <v>18.649999999999999</v>
       </c>
     </row>
     <row r="536" spans="1:6" x14ac:dyDescent="0.2">
@@ -22740,7 +22782,7 @@
         <v>#N/A</v>
       </c>
       <c r="F536">
-        <v>24.03</v>
+        <v>23.81</v>
       </c>
     </row>
     <row r="537" spans="1:6" x14ac:dyDescent="0.2">
@@ -22763,7 +22805,7 @@
         <v>#N/A</v>
       </c>
       <c r="F537">
-        <v>18.98</v>
+        <v>17.88</v>
       </c>
     </row>
     <row r="538" spans="1:6" x14ac:dyDescent="0.2">
@@ -22786,7 +22828,7 @@
         <v>#N/A</v>
       </c>
       <c r="F538">
-        <v>21.659800000000001</v>
+        <v>21</v>
       </c>
     </row>
     <row r="539" spans="1:6" x14ac:dyDescent="0.2">
@@ -22809,7 +22851,7 @@
         <v>#N/A</v>
       </c>
       <c r="F539">
-        <v>25.69</v>
+        <v>25.385000000000002</v>
       </c>
     </row>
     <row r="540" spans="1:6" x14ac:dyDescent="0.2">
@@ -22832,7 +22874,7 @@
         <v>#N/A</v>
       </c>
       <c r="F540">
-        <v>19.23</v>
+        <v>18.579999999999998</v>
       </c>
     </row>
     <row r="541" spans="1:6" x14ac:dyDescent="0.2">
@@ -22901,7 +22943,7 @@
         <v>#N/A</v>
       </c>
       <c r="F543">
-        <v>24.55</v>
+        <v>23.549299999999999</v>
       </c>
     </row>
     <row r="544" spans="1:6" x14ac:dyDescent="0.2">
@@ -22924,7 +22966,7 @@
         <v>#N/A</v>
       </c>
       <c r="F544">
-        <v>17.25</v>
+        <v>15.72</v>
       </c>
     </row>
     <row r="545" spans="1:6" x14ac:dyDescent="0.2">
@@ -22947,7 +22989,7 @@
         <v>#N/A</v>
       </c>
       <c r="F545">
-        <v>19.57</v>
+        <v>19.02</v>
       </c>
     </row>
     <row r="546" spans="1:6" x14ac:dyDescent="0.2">
@@ -22970,7 +23012,7 @@
         <v>#N/A</v>
       </c>
       <c r="F546">
-        <v>17.47</v>
+        <v>17.07</v>
       </c>
     </row>
     <row r="547" spans="1:6" x14ac:dyDescent="0.2">
@@ -22993,7 +23035,7 @@
         <v>#N/A</v>
       </c>
       <c r="F547">
-        <v>19.995000000000001</v>
+        <v>19.741499999999998</v>
       </c>
     </row>
     <row r="548" spans="1:6" x14ac:dyDescent="0.2">
@@ -23016,7 +23058,7 @@
         <v>#N/A</v>
       </c>
       <c r="F548">
-        <v>23.7591</v>
+        <v>23.15</v>
       </c>
     </row>
     <row r="549" spans="1:6" x14ac:dyDescent="0.2">
@@ -23039,7 +23081,7 @@
         <v>#N/A</v>
       </c>
       <c r="F549">
-        <v>4.83</v>
+        <v>4.04</v>
       </c>
     </row>
     <row r="550" spans="1:6" x14ac:dyDescent="0.2">
@@ -23062,7 +23104,7 @@
         <v>#N/A</v>
       </c>
       <c r="F550">
-        <v>19.260000000000002</v>
+        <v>18.684999999999999</v>
       </c>
     </row>
     <row r="551" spans="1:6" x14ac:dyDescent="0.2">
@@ -23085,7 +23127,7 @@
         <v>#N/A</v>
       </c>
       <c r="F551">
-        <v>19.5</v>
+        <v>18.809999999999999</v>
       </c>
     </row>
     <row r="552" spans="1:6" x14ac:dyDescent="0.2">
@@ -23108,7 +23150,7 @@
         <v>#N/A</v>
       </c>
       <c r="F552">
-        <v>20.36</v>
+        <v>18.59</v>
       </c>
     </row>
     <row r="553" spans="1:6" x14ac:dyDescent="0.2">
@@ -23131,7 +23173,7 @@
         <v>#N/A</v>
       </c>
       <c r="F553">
-        <v>17.11</v>
+        <v>16.61</v>
       </c>
     </row>
     <row r="554" spans="1:6" x14ac:dyDescent="0.2">
@@ -23154,7 +23196,7 @@
         <v>#N/A</v>
       </c>
       <c r="F554">
-        <v>20.93</v>
+        <v>20.82</v>
       </c>
     </row>
     <row r="555" spans="1:6" x14ac:dyDescent="0.2">
@@ -23177,7 +23219,7 @@
         <v>#N/A</v>
       </c>
       <c r="F555">
-        <v>19.440000000000001</v>
+        <v>18.23</v>
       </c>
     </row>
     <row r="556" spans="1:6" x14ac:dyDescent="0.2">
@@ -23200,7 +23242,7 @@
         <v>#N/A</v>
       </c>
       <c r="F556">
-        <v>17.57</v>
+        <v>17.350100000000001</v>
       </c>
     </row>
     <row r="557" spans="1:6" x14ac:dyDescent="0.2">
@@ -23223,7 +23265,7 @@
         <v>#N/A</v>
       </c>
       <c r="F557">
-        <v>21.777200000000001</v>
+        <v>21.47</v>
       </c>
     </row>
     <row r="558" spans="1:6" x14ac:dyDescent="0.2">
@@ -23246,7 +23288,7 @@
         <v>#N/A</v>
       </c>
       <c r="F558">
-        <v>24.066199999999998</v>
+        <v>23.76</v>
       </c>
     </row>
     <row r="559" spans="1:6" x14ac:dyDescent="0.2">
@@ -23269,7 +23311,7 @@
         <v>#N/A</v>
       </c>
       <c r="F559">
-        <v>17.8</v>
+        <v>17.52</v>
       </c>
     </row>
     <row r="560" spans="1:6" x14ac:dyDescent="0.2">
@@ -23292,7 +23334,7 @@
         <v>#N/A</v>
       </c>
       <c r="F560">
-        <v>18.1587</v>
+        <v>17.29</v>
       </c>
     </row>
     <row r="561" spans="1:6" x14ac:dyDescent="0.2">
@@ -23315,7 +23357,7 @@
         <v>#N/A</v>
       </c>
       <c r="F561">
-        <v>16.617699999999999</v>
+        <v>15.42</v>
       </c>
     </row>
     <row r="562" spans="1:6" x14ac:dyDescent="0.2">
@@ -23338,7 +23380,7 @@
         <v>#N/A</v>
       </c>
       <c r="F562">
-        <v>16.190000000000001</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="563" spans="1:6" x14ac:dyDescent="0.2">
@@ -23361,7 +23403,7 @@
         <v>#N/A</v>
       </c>
       <c r="F563">
-        <v>16.350000000000001</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="564" spans="1:6" x14ac:dyDescent="0.2">
@@ -23384,7 +23426,7 @@
         <v>#N/A</v>
       </c>
       <c r="F564">
-        <v>18.795000000000002</v>
+        <v>18.16</v>
       </c>
     </row>
     <row r="565" spans="1:6" x14ac:dyDescent="0.2">
@@ -23407,7 +23449,7 @@
         <v>#N/A</v>
       </c>
       <c r="F565">
-        <v>17.899999999999999</v>
+        <v>16.399999999999999</v>
       </c>
     </row>
     <row r="566" spans="1:6" x14ac:dyDescent="0.2">
@@ -23430,7 +23472,7 @@
         <v>#N/A</v>
       </c>
       <c r="F566">
-        <v>18.76125</v>
+        <v>18.039899999999999</v>
       </c>
     </row>
     <row r="567" spans="1:6" x14ac:dyDescent="0.2">
@@ -23453,7 +23495,7 @@
         <v>#N/A</v>
       </c>
       <c r="F567">
-        <v>18.34</v>
+        <v>17.222000000000001</v>
       </c>
     </row>
     <row r="568" spans="1:6" x14ac:dyDescent="0.2">
@@ -23476,7 +23518,7 @@
         <v>#N/A</v>
       </c>
       <c r="F568">
-        <v>22.76</v>
+        <v>23.25</v>
       </c>
     </row>
     <row r="569" spans="1:6" x14ac:dyDescent="0.2">
@@ -23499,7 +23541,7 @@
         <v>#N/A</v>
       </c>
       <c r="F569">
-        <v>24.4315</v>
+        <v>24.51</v>
       </c>
     </row>
     <row r="570" spans="1:6" x14ac:dyDescent="0.2">
@@ -23522,7 +23564,7 @@
         <v>#N/A</v>
       </c>
       <c r="F570">
-        <v>20.63</v>
+        <v>19.920000000000002</v>
       </c>
     </row>
     <row r="571" spans="1:6" x14ac:dyDescent="0.2">
@@ -23568,7 +23610,7 @@
         <v>#N/A</v>
       </c>
       <c r="F572">
-        <v>20.350000000000001</v>
+        <v>18.760000000000002</v>
       </c>
     </row>
     <row r="573" spans="1:6" x14ac:dyDescent="0.2">
@@ -23591,7 +23633,7 @@
         <v>#N/A</v>
       </c>
       <c r="F573">
-        <v>22.379000000000001</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="574" spans="1:6" x14ac:dyDescent="0.2">
@@ -23614,7 +23656,7 @@
         <v>#N/A</v>
       </c>
       <c r="F574">
-        <v>24.7</v>
+        <v>24.21</v>
       </c>
     </row>
     <row r="575" spans="1:6" x14ac:dyDescent="0.2">
@@ -23637,7 +23679,7 @@
         <v>#N/A</v>
       </c>
       <c r="F575">
-        <v>23.33</v>
+        <v>23.09</v>
       </c>
     </row>
     <row r="576" spans="1:6" x14ac:dyDescent="0.2">
@@ -23660,7 +23702,7 @@
         <v>#N/A</v>
       </c>
       <c r="F576">
-        <v>19.3</v>
+        <v>18.55</v>
       </c>
     </row>
     <row r="577" spans="1:6" x14ac:dyDescent="0.2">
@@ -23683,7 +23725,7 @@
         <v>#N/A</v>
       </c>
       <c r="F577">
-        <v>18.579999999999998</v>
+        <v>17.760000000000002</v>
       </c>
     </row>
     <row r="578" spans="1:6" x14ac:dyDescent="0.2">
@@ -23706,7 +23748,7 @@
         <v>#N/A</v>
       </c>
       <c r="F578">
-        <v>17.559999999999999</v>
+        <v>16.579999999999998</v>
       </c>
     </row>
     <row r="579" spans="1:6" x14ac:dyDescent="0.2">
@@ -23729,7 +23771,7 @@
         <v>#N/A</v>
       </c>
       <c r="F579">
-        <v>18.22</v>
+        <v>17.68</v>
       </c>
     </row>
     <row r="580" spans="1:6" x14ac:dyDescent="0.2">
@@ -23752,7 +23794,7 @@
         <v>#N/A</v>
       </c>
       <c r="F580">
-        <v>18.27</v>
+        <v>17.72</v>
       </c>
     </row>
     <row r="581" spans="1:6" x14ac:dyDescent="0.2">
@@ -23775,7 +23817,7 @@
         <v>#N/A</v>
       </c>
       <c r="F581">
-        <v>18.190000000000001</v>
+        <v>17.850000000000001</v>
       </c>
     </row>
     <row r="582" spans="1:6" x14ac:dyDescent="0.2">
@@ -23798,7 +23840,7 @@
         <v>#N/A</v>
       </c>
       <c r="F582">
-        <v>23.26</v>
+        <v>22.28</v>
       </c>
     </row>
     <row r="583" spans="1:6" x14ac:dyDescent="0.2">
@@ -23821,7 +23863,7 @@
         <v>#N/A</v>
       </c>
       <c r="F583">
-        <v>23.3</v>
+        <v>23.545000000000002</v>
       </c>
     </row>
     <row r="584" spans="1:6" x14ac:dyDescent="0.2">
@@ -23844,7 +23886,7 @@
         <v>#N/A</v>
       </c>
       <c r="F584">
-        <v>22.87</v>
+        <v>21.99</v>
       </c>
     </row>
     <row r="585" spans="1:6" x14ac:dyDescent="0.2">
@@ -23867,7 +23909,7 @@
         <v>#N/A</v>
       </c>
       <c r="F585">
-        <v>21.15</v>
+        <v>20.65</v>
       </c>
     </row>
     <row r="586" spans="1:6" x14ac:dyDescent="0.2">
@@ -23890,7 +23932,7 @@
         <v>#N/A</v>
       </c>
       <c r="F586">
-        <v>21.45</v>
+        <v>19.3</v>
       </c>
     </row>
     <row r="587" spans="1:6" x14ac:dyDescent="0.2">
@@ -23913,7 +23955,7 @@
         <v>#N/A</v>
       </c>
       <c r="F587">
-        <v>18.670000000000002</v>
+        <v>17.84</v>
       </c>
     </row>
     <row r="588" spans="1:6" x14ac:dyDescent="0.2">
@@ -23936,7 +23978,7 @@
         <v>#N/A</v>
       </c>
       <c r="F588">
-        <v>19.45</v>
+        <v>18.95</v>
       </c>
     </row>
     <row r="589" spans="1:6" x14ac:dyDescent="0.2">
@@ -23959,7 +24001,7 @@
         <v>#N/A</v>
       </c>
       <c r="F589">
-        <v>20.13</v>
+        <v>19.59</v>
       </c>
     </row>
     <row r="590" spans="1:6" x14ac:dyDescent="0.2">
@@ -23982,7 +24024,7 @@
         <v>#N/A</v>
       </c>
       <c r="F590">
-        <v>24.42</v>
+        <v>24.27</v>
       </c>
     </row>
     <row r="591" spans="1:6" x14ac:dyDescent="0.2">
@@ -24005,7 +24047,7 @@
         <v>#N/A</v>
       </c>
       <c r="F591">
-        <v>24.45</v>
+        <v>24.3</v>
       </c>
     </row>
     <row r="592" spans="1:6" x14ac:dyDescent="0.2">
@@ -24028,7 +24070,7 @@
         <v>#N/A</v>
       </c>
       <c r="F592">
-        <v>24.46</v>
+        <v>24.22</v>
       </c>
     </row>
     <row r="593" spans="1:6" x14ac:dyDescent="0.2">
@@ -24051,7 +24093,7 @@
         <v>#N/A</v>
       </c>
       <c r="F593">
-        <v>91.28</v>
+        <v>90.381799999999998</v>
       </c>
     </row>
     <row r="594" spans="1:6" x14ac:dyDescent="0.2">
@@ -24074,7 +24116,7 @@
         <v>#N/A</v>
       </c>
       <c r="F594">
-        <v>101.11</v>
+        <v>102.52</v>
       </c>
     </row>
     <row r="595" spans="1:6" x14ac:dyDescent="0.2">
@@ -24097,7 +24139,7 @@
         <v>#N/A</v>
       </c>
       <c r="F595">
-        <v>31.16</v>
+        <v>30.31</v>
       </c>
     </row>
     <row r="596" spans="1:6" x14ac:dyDescent="0.2">
@@ -24120,7 +24162,7 @@
         <v>#N/A</v>
       </c>
       <c r="F596">
-        <v>20.65</v>
+        <v>20.0793</v>
       </c>
     </row>
     <row r="597" spans="1:6" x14ac:dyDescent="0.2">
@@ -24143,7 +24185,7 @@
         <v>#N/A</v>
       </c>
       <c r="F597">
-        <v>18.52</v>
+        <v>17.920000000000002</v>
       </c>
     </row>
     <row r="598" spans="1:6" x14ac:dyDescent="0.2">
@@ -24166,7 +24208,7 @@
         <v>#N/A</v>
       </c>
       <c r="F598">
-        <v>16.420000000000002</v>
+        <v>15.31</v>
       </c>
     </row>
     <row r="599" spans="1:6" x14ac:dyDescent="0.2">
@@ -24189,7 +24231,7 @@
         <v>#N/A</v>
       </c>
       <c r="F599" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="600" spans="1:6" x14ac:dyDescent="0.2">
@@ -24212,7 +24254,7 @@
         <v>#N/A</v>
       </c>
       <c r="F600">
-        <v>24.232500000000002</v>
+        <v>23.779800000000002</v>
       </c>
     </row>
     <row r="601" spans="1:6" x14ac:dyDescent="0.2">
@@ -24235,7 +24277,7 @@
         <v>#N/A</v>
       </c>
       <c r="F601">
-        <v>22.05</v>
+        <v>22.19</v>
       </c>
     </row>
     <row r="602" spans="1:6" x14ac:dyDescent="0.2">
@@ -24258,7 +24300,7 @@
         <v>#N/A</v>
       </c>
       <c r="F602">
-        <v>27.797599999999999</v>
+        <v>27.7</v>
       </c>
     </row>
     <row r="603" spans="1:6" x14ac:dyDescent="0.2">
@@ -24281,7 +24323,7 @@
         <v>#N/A</v>
       </c>
       <c r="F603">
-        <v>24.33</v>
+        <v>22.9</v>
       </c>
     </row>
     <row r="604" spans="1:6" x14ac:dyDescent="0.2">
@@ -24304,7 +24346,7 @@
         <v>#N/A</v>
       </c>
       <c r="F604">
-        <v>17.060400000000001</v>
+        <v>16</v>
       </c>
     </row>
     <row r="605" spans="1:6" x14ac:dyDescent="0.2">
@@ -24327,7 +24369,7 @@
         <v>#N/A</v>
       </c>
       <c r="F605">
-        <v>21.7</v>
+        <v>20.78</v>
       </c>
     </row>
     <row r="606" spans="1:6" x14ac:dyDescent="0.2">
@@ -24350,7 +24392,7 @@
         <v>#N/A</v>
       </c>
       <c r="F606">
-        <v>21.56</v>
+        <v>20.64</v>
       </c>
     </row>
     <row r="607" spans="1:6" x14ac:dyDescent="0.2">
@@ -24373,7 +24415,7 @@
         <v>#N/A</v>
       </c>
       <c r="F607">
-        <v>20.86</v>
+        <v>19.3</v>
       </c>
     </row>
     <row r="608" spans="1:6" x14ac:dyDescent="0.2">
@@ -24396,7 +24438,7 @@
         <v>#N/A</v>
       </c>
       <c r="F608">
-        <v>18.89</v>
+        <v>17.09</v>
       </c>
     </row>
     <row r="609" spans="1:6" x14ac:dyDescent="0.2">
@@ -24419,7 +24461,7 @@
         <v>#N/A</v>
       </c>
       <c r="F609">
-        <v>16.37</v>
+        <v>16.45</v>
       </c>
     </row>
     <row r="610" spans="1:6" x14ac:dyDescent="0.2">
@@ -24442,7 +24484,7 @@
         <v>#N/A</v>
       </c>
       <c r="F610">
-        <v>19.149999999999999</v>
+        <v>18.84</v>
       </c>
     </row>
     <row r="611" spans="1:6" x14ac:dyDescent="0.2">
@@ -24465,7 +24507,7 @@
         <v>#N/A</v>
       </c>
       <c r="F611">
-        <v>18.22</v>
+        <v>17.149999999999999</v>
       </c>
     </row>
     <row r="612" spans="1:6" x14ac:dyDescent="0.2">
@@ -24488,7 +24530,7 @@
         <v>#N/A</v>
       </c>
       <c r="F612">
-        <v>18.13</v>
+        <v>17.75</v>
       </c>
     </row>
     <row r="613" spans="1:6" x14ac:dyDescent="0.2">
@@ -24511,7 +24553,7 @@
         <v>#N/A</v>
       </c>
       <c r="F613">
-        <v>20.47</v>
+        <v>19.93</v>
       </c>
     </row>
     <row r="614" spans="1:6" x14ac:dyDescent="0.2">
@@ -24534,7 +24576,7 @@
         <v>#N/A</v>
       </c>
       <c r="F614">
-        <v>19.920000000000002</v>
+        <v>19.11</v>
       </c>
     </row>
     <row r="615" spans="1:6" x14ac:dyDescent="0.2">
@@ -24557,7 +24599,7 @@
         <v>#N/A</v>
       </c>
       <c r="F615">
-        <v>23.013100000000001</v>
+        <v>22.27</v>
       </c>
     </row>
     <row r="616" spans="1:6" x14ac:dyDescent="0.2">
@@ -24580,7 +24622,7 @@
         <v>#N/A</v>
       </c>
       <c r="F616">
-        <v>25.16</v>
+        <v>25.37</v>
       </c>
     </row>
     <row r="617" spans="1:6" x14ac:dyDescent="0.2">
@@ -24603,7 +24645,7 @@
         <v>#N/A</v>
       </c>
       <c r="F617">
-        <v>21.38</v>
+        <v>20.8</v>
       </c>
     </row>
     <row r="618" spans="1:6" x14ac:dyDescent="0.2">
@@ -24626,7 +24668,7 @@
         <v>#N/A</v>
       </c>
       <c r="F618">
-        <v>21.29</v>
+        <v>20.96</v>
       </c>
     </row>
     <row r="619" spans="1:6" x14ac:dyDescent="0.2">
@@ -24649,7 +24691,7 @@
         <v>#N/A</v>
       </c>
       <c r="F619">
-        <v>21.5</v>
+        <v>20.94</v>
       </c>
     </row>
     <row r="620" spans="1:6" x14ac:dyDescent="0.2">
@@ -24672,7 +24714,7 @@
         <v>#N/A</v>
       </c>
       <c r="F620">
-        <v>49.2</v>
+        <v>45.475000000000001</v>
       </c>
     </row>
     <row r="621" spans="1:6" x14ac:dyDescent="0.2">
@@ -24695,7 +24737,7 @@
         <v>#N/A</v>
       </c>
       <c r="F621">
-        <v>18.27</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="622" spans="1:6" x14ac:dyDescent="0.2">
@@ -24718,7 +24760,7 @@
         <v>#N/A</v>
       </c>
       <c r="F622">
-        <v>19.13</v>
+        <v>18.47</v>
       </c>
     </row>
     <row r="623" spans="1:6" x14ac:dyDescent="0.2">
@@ -24741,7 +24783,7 @@
         <v>#N/A</v>
       </c>
       <c r="F623">
-        <v>19.350000000000001</v>
+        <v>18.8</v>
       </c>
     </row>
     <row r="624" spans="1:6" x14ac:dyDescent="0.2">
@@ -24764,7 +24806,7 @@
         <v>#N/A</v>
       </c>
       <c r="F624">
-        <v>19.16</v>
+        <v>18.239999999999998</v>
       </c>
     </row>
     <row r="625" spans="1:6" x14ac:dyDescent="0.2">
@@ -24787,7 +24829,7 @@
         <v>#N/A</v>
       </c>
       <c r="F625">
-        <v>18.96</v>
+        <v>18.45</v>
       </c>
     </row>
     <row r="626" spans="1:6" x14ac:dyDescent="0.2">
@@ -24833,7 +24875,7 @@
         <v>#N/A</v>
       </c>
       <c r="F627">
-        <v>20.2</v>
+        <v>19.9999</v>
       </c>
     </row>
     <row r="628" spans="1:6" x14ac:dyDescent="0.2">
@@ -24856,7 +24898,7 @@
         <v>#N/A</v>
       </c>
       <c r="F628">
-        <v>20.149899999999999</v>
+        <v>19.68</v>
       </c>
     </row>
     <row r="629" spans="1:6" x14ac:dyDescent="0.2">
@@ -24879,7 +24921,7 @@
         <v>#N/A</v>
       </c>
       <c r="F629">
-        <v>20.25</v>
+        <v>19.899999999999999</v>
       </c>
     </row>
     <row r="630" spans="1:6" x14ac:dyDescent="0.2">
@@ -24902,7 +24944,7 @@
         <v>#N/A</v>
       </c>
       <c r="F630">
-        <v>19.010000000000002</v>
+        <v>18.399999999999999</v>
       </c>
     </row>
     <row r="631" spans="1:6" x14ac:dyDescent="0.2">
@@ -24925,7 +24967,7 @@
         <v>#N/A</v>
       </c>
       <c r="F631">
-        <v>19.989999999999998</v>
+        <v>19.98</v>
       </c>
     </row>
     <row r="632" spans="1:6" x14ac:dyDescent="0.2">
@@ -24948,7 +24990,7 @@
         <v>#N/A</v>
       </c>
       <c r="F632">
-        <v>18.960599999999999</v>
+        <v>18.600100000000001</v>
       </c>
     </row>
     <row r="633" spans="1:6" x14ac:dyDescent="0.2">
@@ -24971,7 +25013,7 @@
         <v>#N/A</v>
       </c>
       <c r="F633">
-        <v>18.45</v>
+        <v>18.170000000000002</v>
       </c>
     </row>
     <row r="634" spans="1:6" x14ac:dyDescent="0.2">
@@ -24994,7 +25036,7 @@
         <v>#N/A</v>
       </c>
       <c r="F634">
-        <v>21.34</v>
+        <v>20.010000000000002</v>
       </c>
     </row>
     <row r="635" spans="1:6" x14ac:dyDescent="0.2">
@@ -25017,7 +25059,7 @@
         <v>#N/A</v>
       </c>
       <c r="F635">
-        <v>84.11</v>
+        <v>83.54</v>
       </c>
     </row>
     <row r="636" spans="1:6" x14ac:dyDescent="0.2">
@@ -25040,7 +25082,7 @@
         <v>#N/A</v>
       </c>
       <c r="F636">
-        <v>24.54</v>
+        <v>23.72</v>
       </c>
     </row>
     <row r="637" spans="1:6" x14ac:dyDescent="0.2">
@@ -25063,7 +25105,7 @@
         <v>#N/A</v>
       </c>
       <c r="F637">
-        <v>16.840699999999998</v>
+        <v>15.73</v>
       </c>
     </row>
     <row r="638" spans="1:6" x14ac:dyDescent="0.2">
@@ -25086,7 +25128,7 @@
         <v>#N/A</v>
       </c>
       <c r="F638">
-        <v>19.329999999999998</v>
+        <v>18.850000000000001</v>
       </c>
     </row>
     <row r="639" spans="1:6" x14ac:dyDescent="0.2">
@@ -25109,7 +25151,7 @@
         <v>#N/A</v>
       </c>
       <c r="F639">
-        <v>17.149999999999999</v>
+        <v>16.86</v>
       </c>
     </row>
     <row r="640" spans="1:6" x14ac:dyDescent="0.2">
@@ -25132,7 +25174,7 @@
         <v>#N/A</v>
       </c>
       <c r="F640">
-        <v>16.97</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="641" spans="1:6" x14ac:dyDescent="0.2">
@@ -25155,7 +25197,7 @@
         <v>#N/A</v>
       </c>
       <c r="F641">
-        <v>26.74</v>
+        <v>26.78</v>
       </c>
     </row>
     <row r="642" spans="1:6" x14ac:dyDescent="0.2">
@@ -25178,7 +25220,7 @@
         <v>#N/A</v>
       </c>
       <c r="F642">
-        <v>17.049900000000001</v>
+        <v>16.59</v>
       </c>
     </row>
     <row r="643" spans="1:6" x14ac:dyDescent="0.2">
@@ -25201,7 +25243,7 @@
         <v>#N/A</v>
       </c>
       <c r="F643">
-        <v>18.78</v>
+        <v>18.3</v>
       </c>
     </row>
     <row r="644" spans="1:6" x14ac:dyDescent="0.2">
@@ -25224,7 +25266,7 @@
         <v>#N/A</v>
       </c>
       <c r="F644">
-        <v>18.11</v>
+        <v>17.579999999999998</v>
       </c>
     </row>
     <row r="645" spans="1:6" x14ac:dyDescent="0.2">
@@ -25247,7 +25289,7 @@
         <v>#N/A</v>
       </c>
       <c r="F645">
-        <v>16.8</v>
+        <v>15.93</v>
       </c>
     </row>
     <row r="646" spans="1:6" x14ac:dyDescent="0.2">
@@ -25270,7 +25312,7 @@
         <v>#N/A</v>
       </c>
       <c r="F646">
-        <v>18.13</v>
+        <v>16.100000000000001</v>
       </c>
     </row>
     <row r="647" spans="1:6" x14ac:dyDescent="0.2">
@@ -25293,7 +25335,7 @@
         <v>#N/A</v>
       </c>
       <c r="F647">
-        <v>17.89</v>
+        <v>17.43</v>
       </c>
     </row>
     <row r="648" spans="1:6" x14ac:dyDescent="0.2">
@@ -25316,7 +25358,7 @@
         <v>#N/A</v>
       </c>
       <c r="F648">
-        <v>18.39</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="649" spans="1:6" x14ac:dyDescent="0.2">
@@ -25339,7 +25381,7 @@
         <v>#N/A</v>
       </c>
       <c r="F649">
-        <v>18.73</v>
+        <v>17.350000000000001</v>
       </c>
     </row>
     <row r="650" spans="1:6" x14ac:dyDescent="0.2">
@@ -25362,7 +25404,7 @@
         <v>#N/A</v>
       </c>
       <c r="F650">
-        <v>8.93</v>
+        <v>8.25</v>
       </c>
     </row>
     <row r="651" spans="1:6" x14ac:dyDescent="0.2">
@@ -25385,7 +25427,7 @@
         <v>#N/A</v>
       </c>
       <c r="F651">
-        <v>20.71</v>
+        <v>20.34</v>
       </c>
     </row>
     <row r="652" spans="1:6" x14ac:dyDescent="0.2">
@@ -25408,7 +25450,7 @@
         <v>#N/A</v>
       </c>
       <c r="F652">
-        <v>21.4</v>
+        <v>19.89</v>
       </c>
     </row>
     <row r="653" spans="1:6" x14ac:dyDescent="0.2">
@@ -25431,7 +25473,7 @@
         <v>#N/A</v>
       </c>
       <c r="F653">
-        <v>19</v>
+        <v>18.399999999999999</v>
       </c>
     </row>
     <row r="654" spans="1:6" x14ac:dyDescent="0.2">
@@ -25454,7 +25496,7 @@
         <v>#N/A</v>
       </c>
       <c r="F654">
-        <v>17.61</v>
+        <v>17.16</v>
       </c>
     </row>
     <row r="655" spans="1:6" x14ac:dyDescent="0.2">
@@ -25477,7 +25519,7 @@
         <v>#N/A</v>
       </c>
       <c r="F655">
-        <v>19.43</v>
+        <v>18.05</v>
       </c>
     </row>
     <row r="656" spans="1:6" x14ac:dyDescent="0.2">
@@ -25500,7 +25542,7 @@
         <v>#N/A</v>
       </c>
       <c r="F656">
-        <v>13.02</v>
+        <v>14.66</v>
       </c>
     </row>
     <row r="657" spans="1:6" x14ac:dyDescent="0.2">
@@ -25523,7 +25565,7 @@
         <v>#N/A</v>
       </c>
       <c r="F657">
-        <v>21.109375</v>
+        <v>20.51</v>
       </c>
     </row>
     <row r="658" spans="1:6" x14ac:dyDescent="0.2">
@@ -25546,7 +25588,7 @@
         <v>#N/A</v>
       </c>
       <c r="F658">
-        <v>18.649999999999999</v>
+        <v>17.98</v>
       </c>
     </row>
     <row r="659" spans="1:6" x14ac:dyDescent="0.2">
@@ -25569,7 +25611,7 @@
         <v>#N/A</v>
       </c>
       <c r="F659">
-        <v>21.34</v>
+        <v>20.350000000000001</v>
       </c>
     </row>
     <row r="660" spans="1:6" x14ac:dyDescent="0.2">
@@ -25592,7 +25634,7 @@
         <v>#N/A</v>
       </c>
       <c r="F660">
-        <v>21.08</v>
+        <v>20.73</v>
       </c>
     </row>
     <row r="661" spans="1:6" x14ac:dyDescent="0.2">
@@ -25615,7 +25657,7 @@
         <v>#N/A</v>
       </c>
       <c r="F661">
-        <v>19.728300000000001</v>
+        <v>18.010000000000002</v>
       </c>
     </row>
     <row r="662" spans="1:6" x14ac:dyDescent="0.2">
@@ -25638,7 +25680,7 @@
         <v>#N/A</v>
       </c>
       <c r="F662">
-        <v>17.55</v>
+        <v>17.2</v>
       </c>
     </row>
     <row r="663" spans="1:6" x14ac:dyDescent="0.2">
@@ -25661,7 +25703,7 @@
         <v>#N/A</v>
       </c>
       <c r="F663">
-        <v>24.085000000000001</v>
+        <v>24.38</v>
       </c>
     </row>
     <row r="664" spans="1:6" x14ac:dyDescent="0.2">
@@ -25684,7 +25726,7 @@
         <v>#N/A</v>
       </c>
       <c r="F664">
-        <v>21.5</v>
+        <v>20.645</v>
       </c>
     </row>
     <row r="665" spans="1:6" x14ac:dyDescent="0.2">
@@ -25707,7 +25749,7 @@
         <v>#N/A</v>
       </c>
       <c r="F665">
-        <v>10.66</v>
+        <v>10.29</v>
       </c>
     </row>
     <row r="666" spans="1:6" x14ac:dyDescent="0.2">
@@ -25730,7 +25772,7 @@
         <v>#N/A</v>
       </c>
       <c r="F666">
-        <v>20.84</v>
+        <v>19.57</v>
       </c>
     </row>
     <row r="667" spans="1:6" x14ac:dyDescent="0.2">
@@ -25753,7 +25795,7 @@
         <v>#N/A</v>
       </c>
       <c r="F667">
-        <v>112.21</v>
+        <v>114.5959</v>
       </c>
     </row>
     <row r="668" spans="1:6" x14ac:dyDescent="0.2">
@@ -25776,7 +25818,7 @@
         <v>#N/A</v>
       </c>
       <c r="F668">
-        <v>14.17</v>
+        <v>13.39</v>
       </c>
     </row>
     <row r="669" spans="1:6" x14ac:dyDescent="0.2">
@@ -25799,7 +25841,7 @@
         <v>#N/A</v>
       </c>
       <c r="F669">
-        <v>20.91</v>
+        <v>18.920000000000002</v>
       </c>
     </row>
     <row r="670" spans="1:6" x14ac:dyDescent="0.2">
@@ -25822,7 +25864,7 @@
         <v>#N/A</v>
       </c>
       <c r="F670">
-        <v>21.637599999999999</v>
+        <v>20.52</v>
       </c>
     </row>
     <row r="671" spans="1:6" x14ac:dyDescent="0.2">
@@ -25845,7 +25887,7 @@
         <v>#N/A</v>
       </c>
       <c r="F671">
-        <v>18.68</v>
+        <v>18.239999999999998</v>
       </c>
     </row>
     <row r="672" spans="1:6" x14ac:dyDescent="0.2">
@@ -25868,7 +25910,7 @@
         <v>#N/A</v>
       </c>
       <c r="F672">
-        <v>18.46</v>
+        <v>17.920000000000002</v>
       </c>
     </row>
     <row r="673" spans="1:6" x14ac:dyDescent="0.2">
@@ -25891,7 +25933,7 @@
         <v>#N/A</v>
       </c>
       <c r="F673">
-        <v>18.059999999999999</v>
+        <v>17.484999999999999</v>
       </c>
     </row>
     <row r="674" spans="1:6" x14ac:dyDescent="0.2">
@@ -25914,7 +25956,7 @@
         <v>#N/A</v>
       </c>
       <c r="F674">
-        <v>14</v>
+        <v>13.37</v>
       </c>
     </row>
     <row r="675" spans="1:6" x14ac:dyDescent="0.2">
@@ -25937,7 +25979,7 @@
         <v>#N/A</v>
       </c>
       <c r="F675">
-        <v>17.850000000000001</v>
+        <v>16.39</v>
       </c>
     </row>
     <row r="676" spans="1:6" x14ac:dyDescent="0.2">
@@ -25960,7 +26002,7 @@
         <v>#N/A</v>
       </c>
       <c r="F676">
-        <v>17.93</v>
+        <v>16.760000000000002</v>
       </c>
     </row>
     <row r="677" spans="1:6" x14ac:dyDescent="0.2">
@@ -25983,7 +26025,7 @@
         <v>#N/A</v>
       </c>
       <c r="F677">
-        <v>20.190000000000001</v>
+        <v>19.37</v>
       </c>
     </row>
     <row r="678" spans="1:6" x14ac:dyDescent="0.2">
@@ -26006,7 +26048,7 @@
         <v>#N/A</v>
       </c>
       <c r="F678">
-        <v>17.52</v>
+        <v>16.86</v>
       </c>
     </row>
     <row r="679" spans="1:6" x14ac:dyDescent="0.2">
@@ -26029,7 +26071,7 @@
         <v>#N/A</v>
       </c>
       <c r="F679">
-        <v>22.8</v>
+        <v>22.790900000000001</v>
       </c>
     </row>
     <row r="680" spans="1:6" x14ac:dyDescent="0.2">
@@ -26052,7 +26094,7 @@
         <v>#N/A</v>
       </c>
       <c r="F680">
-        <v>23.66</v>
+        <v>23.7257</v>
       </c>
     </row>
     <row r="681" spans="1:6" x14ac:dyDescent="0.2">
@@ -26075,7 +26117,7 @@
         <v>#N/A</v>
       </c>
       <c r="F681">
-        <v>18.440000000000001</v>
+        <v>17.23</v>
       </c>
     </row>
     <row r="682" spans="1:6" x14ac:dyDescent="0.2">
@@ -26098,7 +26140,7 @@
         <v>#N/A</v>
       </c>
       <c r="F682">
-        <v>20.89</v>
+        <v>20</v>
       </c>
     </row>
     <row r="683" spans="1:6" x14ac:dyDescent="0.2">
@@ -26121,7 +26163,7 @@
         <v>#N/A</v>
       </c>
       <c r="F683">
-        <v>17.350000000000001</v>
+        <v>15.67</v>
       </c>
     </row>
     <row r="684" spans="1:6" x14ac:dyDescent="0.2">
@@ -26144,7 +26186,7 @@
         <v>#N/A</v>
       </c>
       <c r="F684">
-        <v>22.12</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="685" spans="1:6" x14ac:dyDescent="0.2">
@@ -26167,7 +26209,7 @@
         <v>#N/A</v>
       </c>
       <c r="F685">
-        <v>20.03</v>
+        <v>19.649999999999999</v>
       </c>
     </row>
     <row r="686" spans="1:6" x14ac:dyDescent="0.2">
@@ -26190,7 +26232,7 @@
         <v>#N/A</v>
       </c>
       <c r="F686">
-        <v>21.8</v>
+        <v>21.53</v>
       </c>
     </row>
     <row r="687" spans="1:6" x14ac:dyDescent="0.2">
@@ -26213,7 +26255,7 @@
         <v>#N/A</v>
       </c>
       <c r="F687">
-        <v>18.829999999999998</v>
+        <v>18.170000000000002</v>
       </c>
     </row>
     <row r="688" spans="1:6" x14ac:dyDescent="0.2">
@@ -26236,7 +26278,7 @@
         <v>#N/A</v>
       </c>
       <c r="F688">
-        <v>19.25</v>
+        <v>17.14</v>
       </c>
     </row>
     <row r="689" spans="1:6" x14ac:dyDescent="0.2">
@@ -26259,7 +26301,7 @@
         <v>#N/A</v>
       </c>
       <c r="F689">
-        <v>18.245000000000001</v>
+        <v>17.64</v>
       </c>
     </row>
     <row r="690" spans="1:6" x14ac:dyDescent="0.2">
@@ -26282,7 +26324,7 @@
         <v>#N/A</v>
       </c>
       <c r="F690">
-        <v>25</v>
+        <v>24.532299999999999</v>
       </c>
     </row>
     <row r="691" spans="1:6" x14ac:dyDescent="0.2">
@@ -26305,7 +26347,7 @@
         <v>#N/A</v>
       </c>
       <c r="F691">
-        <v>25.1</v>
+        <v>24.86</v>
       </c>
     </row>
     <row r="692" spans="1:6" x14ac:dyDescent="0.2">
@@ -26328,7 +26370,7 @@
         <v>#N/A</v>
       </c>
       <c r="F692">
-        <v>25.23</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="693" spans="1:6" x14ac:dyDescent="0.2">
@@ -26351,7 +26393,7 @@
         <v>#N/A</v>
       </c>
       <c r="F693">
-        <v>20.54</v>
+        <v>20.02</v>
       </c>
     </row>
     <row r="694" spans="1:6" x14ac:dyDescent="0.2">
@@ -26374,7 +26416,7 @@
         <v>#N/A</v>
       </c>
       <c r="F694">
-        <v>20.22</v>
+        <v>19.649999999999999</v>
       </c>
     </row>
     <row r="695" spans="1:6" x14ac:dyDescent="0.2">
@@ -26397,7 +26439,7 @@
         <v>#N/A</v>
       </c>
       <c r="F695">
-        <v>20.52</v>
+        <v>19.98</v>
       </c>
     </row>
     <row r="696" spans="1:6" x14ac:dyDescent="0.2">
@@ -26420,7 +26462,7 @@
         <v>#N/A</v>
       </c>
       <c r="F696">
-        <v>25.49</v>
+        <v>25.4499</v>
       </c>
     </row>
     <row r="697" spans="1:6" x14ac:dyDescent="0.2">
@@ -26443,7 +26485,7 @@
         <v>#N/A</v>
       </c>
       <c r="F697">
-        <v>24.87</v>
+        <v>24.436399999999999</v>
       </c>
     </row>
     <row r="698" spans="1:6" x14ac:dyDescent="0.2">
@@ -26466,7 +26508,7 @@
         <v>#N/A</v>
       </c>
       <c r="F698">
-        <v>15.61</v>
+        <v>15.82</v>
       </c>
     </row>
     <row r="699" spans="1:6" x14ac:dyDescent="0.2">
@@ -26489,7 +26531,7 @@
         <v>#N/A</v>
       </c>
       <c r="F699">
-        <v>25.437999999999999</v>
+        <v>24.65</v>
       </c>
     </row>
     <row r="700" spans="1:6" x14ac:dyDescent="0.2">
@@ -26512,7 +26554,7 @@
         <v>#N/A</v>
       </c>
       <c r="F700">
-        <v>2.09</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="701" spans="1:6" x14ac:dyDescent="0.2">
@@ -26535,7 +26577,7 @@
         <v>#N/A</v>
       </c>
       <c r="F701">
-        <v>25.59</v>
+        <v>25.43</v>
       </c>
     </row>
     <row r="702" spans="1:6" x14ac:dyDescent="0.2">
@@ -26558,7 +26600,7 @@
         <v>#N/A</v>
       </c>
       <c r="F702">
-        <v>24.74</v>
+        <v>24.24</v>
       </c>
     </row>
     <row r="703" spans="1:6" x14ac:dyDescent="0.2">
@@ -26581,7 +26623,7 @@
         <v>#N/A</v>
       </c>
       <c r="F703">
-        <v>24.38</v>
+        <v>23.67</v>
       </c>
     </row>
     <row r="704" spans="1:6" x14ac:dyDescent="0.2">
@@ -26604,7 +26646,7 @@
         <v>#N/A</v>
       </c>
       <c r="F704">
-        <v>25.14</v>
+        <v>24.91</v>
       </c>
     </row>
     <row r="705" spans="1:6" x14ac:dyDescent="0.2">
@@ -26627,7 +26669,7 @@
         <v>#N/A</v>
       </c>
       <c r="F705">
-        <v>25.1175</v>
+        <v>25.2499</v>
       </c>
     </row>
     <row r="706" spans="1:6" x14ac:dyDescent="0.2">
@@ -26650,7 +26692,7 @@
         <v>#N/A</v>
       </c>
       <c r="F706">
-        <v>593.57000000000005</v>
+        <v>622.52</v>
       </c>
     </row>
     <row r="707" spans="1:6" x14ac:dyDescent="0.2">
@@ -26661,11 +26703,11 @@
         <v>1404</v>
       </c>
       <c r="C707" t="str">
-        <f t="shared" ref="C707:C716" si="22">SUBSTITUTE(B707,".PR","p")</f>
+        <f t="shared" ref="C707:C719" si="22">SUBSTITUTE(B707,".PR","p")</f>
         <v>MBINM</v>
       </c>
       <c r="D707" t="str">
-        <f t="shared" ref="D707:D716" si="23">SUBSTITUTE(B707,".PR"," ")&amp;" Pfd"</f>
+        <f t="shared" ref="D707:D719" si="23">SUBSTITUTE(B707,".PR"," ")&amp;" Pfd"</f>
         <v>MBINM Pfd</v>
       </c>
       <c r="E707" t="e">
@@ -26673,7 +26715,7 @@
         <v>#N/A</v>
       </c>
       <c r="F707">
-        <v>27.125</v>
+        <v>26.2</v>
       </c>
     </row>
     <row r="708" spans="1:6" x14ac:dyDescent="0.2">
@@ -26696,7 +26738,7 @@
         <v>#N/A</v>
       </c>
       <c r="F708">
-        <v>22.65</v>
+        <v>22.56</v>
       </c>
     </row>
     <row r="709" spans="1:6" x14ac:dyDescent="0.2">
@@ -26719,7 +26761,7 @@
         <v>#N/A</v>
       </c>
       <c r="F709">
-        <v>26.460799999999999</v>
+        <v>25.950099999999999</v>
       </c>
     </row>
     <row r="710" spans="1:6" x14ac:dyDescent="0.2">
@@ -26742,7 +26784,7 @@
         <v>#N/A</v>
       </c>
       <c r="F710">
-        <v>43.67</v>
+        <v>45.18</v>
       </c>
     </row>
     <row r="711" spans="1:6" x14ac:dyDescent="0.2">
@@ -26765,7 +26807,7 @@
         <v>#N/A</v>
       </c>
       <c r="F711">
-        <v>26.15</v>
+        <v>26.41</v>
       </c>
     </row>
     <row r="712" spans="1:6" x14ac:dyDescent="0.2">
@@ -26788,7 +26830,7 @@
         <v>#N/A</v>
       </c>
       <c r="F712">
-        <v>18.2</v>
+        <v>16.89</v>
       </c>
     </row>
     <row r="713" spans="1:6" x14ac:dyDescent="0.2">
@@ -26811,7 +26853,7 @@
         <v>#N/A</v>
       </c>
       <c r="F713">
-        <v>55.93</v>
+        <v>59.69</v>
       </c>
     </row>
     <row r="714" spans="1:6" x14ac:dyDescent="0.2">
@@ -26834,7 +26876,7 @@
         <v>#N/A</v>
       </c>
       <c r="F714">
-        <v>26.26</v>
+        <v>26.35</v>
       </c>
     </row>
     <row r="715" spans="1:6" x14ac:dyDescent="0.2">
@@ -26857,7 +26899,7 @@
         <v>#N/A</v>
       </c>
       <c r="F715">
-        <v>27.74</v>
+        <v>27.79</v>
       </c>
     </row>
     <row r="716" spans="1:6" x14ac:dyDescent="0.2">
@@ -26880,7 +26922,76 @@
         <v>#N/A</v>
       </c>
       <c r="F716">
-        <v>24.36</v>
+        <v>23.77</v>
+      </c>
+    </row>
+    <row r="717" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A717" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B717" t="s">
+        <v>1437</v>
+      </c>
+      <c r="C717" t="str">
+        <f t="shared" si="22"/>
+        <v>ASBA</v>
+      </c>
+      <c r="D717" t="str">
+        <f t="shared" si="23"/>
+        <v>ASBA Pfd</v>
+      </c>
+      <c r="E717" t="e">
+        <f>RTD("activrtd","","realtime",C717,"Last(0,12;0,113)")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F717">
+        <v>25.15</v>
+      </c>
+    </row>
+    <row r="718" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A718" t="s">
+        <v>1442</v>
+      </c>
+      <c r="B718" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C718" t="str">
+        <f t="shared" si="22"/>
+        <v>HBANL</v>
+      </c>
+      <c r="D718" t="str">
+        <f t="shared" si="23"/>
+        <v>HBANL Pfd</v>
+      </c>
+      <c r="E718" t="e">
+        <f>RTD("activrtd","","realtime",C718,"Last(0,12;0,113)")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F718">
+        <v>24.81</v>
+      </c>
+    </row>
+    <row r="719" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A719" t="s">
+        <v>1440</v>
+      </c>
+      <c r="B719" t="s">
+        <v>1441</v>
+      </c>
+      <c r="C719" t="str">
+        <f t="shared" si="22"/>
+        <v>CEQPp</v>
+      </c>
+      <c r="D719" t="str">
+        <f t="shared" si="23"/>
+        <v>CEQP  Pfd</v>
+      </c>
+      <c r="E719" t="e">
+        <f>RTD("activrtd","","realtime",C719,"Last(0,12;0,113)")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F719">
+        <v>9.06</v>
       </c>
     </row>
     <row r="1256" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>